<commit_message>
add some code on data loading at run.py
</commit_message>
<xml_diff>
--- a/numbers.xlsx
+++ b/numbers.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stratos/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0536E6-863A-8A48-B180-6D4FB13AE1E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{36369E5E-9824-0C46-B465-B8650ED0CAC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{3334AC23-09C0-AC47-B60F-5D2A5875DA56}"/>
+    <workbookView xWindow="8380" yWindow="4720" windowWidth="28040" windowHeight="17440" xr2:uid="{3334AC23-09C0-AC47-B60F-5D2A5875DA56}"/>
   </bookViews>
   <sheets>
     <sheet name="random numbers" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,6 +37,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -66,9 +69,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,2975 +387,3165 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F2E5948-90E8-8C4F-BB3E-A91504EAC9A5}">
-  <dimension ref="A1:O63"/>
+  <dimension ref="A1:P63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="1">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="2">
+        <v>45002</v>
+      </c>
+      <c r="B1" s="1">
         <v>0.50409909202549374</v>
       </c>
-      <c r="B1" s="1">
+      <c r="C1" s="1">
         <v>0.94638479100675488</v>
       </c>
-      <c r="C1" s="1">
+      <c r="D1" s="1">
         <v>0.94505032374366715</v>
       </c>
-      <c r="D1" s="1">
+      <c r="E1" s="1">
         <v>8.4574897272943428E-2</v>
       </c>
-      <c r="E1" s="1">
+      <c r="F1" s="1">
         <v>0.8154458174317587</v>
       </c>
-      <c r="F1" s="1">
+      <c r="G1" s="1">
         <v>0.61069917956830733</v>
       </c>
-      <c r="G1" s="1">
+      <c r="H1" s="1">
         <v>0.50967514067926845</v>
       </c>
-      <c r="H1" s="1">
+      <c r="I1" s="1">
         <v>0.57829194012792895</v>
       </c>
-      <c r="I1" s="1">
+      <c r="J1" s="1">
         <v>7.7586580471318833E-2</v>
       </c>
-      <c r="J1" s="1">
+      <c r="K1" s="1">
         <v>0.85350248734684819</v>
       </c>
-      <c r="K1" s="1">
+      <c r="L1" s="1">
         <v>0.27406197951488498</v>
       </c>
-      <c r="L1" s="1">
+      <c r="M1" s="1">
         <v>0.60036797214520776</v>
       </c>
-      <c r="M1" s="1">
+      <c r="N1" s="1">
         <v>0.63644143610209547</v>
       </c>
-      <c r="N1" s="1">
+      <c r="O1" s="1">
         <v>0.1919979528484872</v>
       </c>
-      <c r="O1" s="1">
+      <c r="P1" s="1">
         <v>0.42572234555476285</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>45001</v>
+      </c>
+      <c r="B2" s="1">
         <v>0.22892362540086841</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2" s="1">
         <v>0.70235074437485256</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>0.79906198965262942</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>0.97829452705063447</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>7.9178451105004322E-2</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>0.61663853244070665</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>0.16305217931665017</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>0.56082214733976854</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2" s="1">
         <v>0.64183507857497413</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>0.97911562089086601</v>
       </c>
-      <c r="K2" s="1">
+      <c r="L2" s="1">
         <v>9.7568811095803287E-2</v>
       </c>
-      <c r="L2" s="1">
+      <c r="M2" s="1">
         <v>0.17851234447365028</v>
       </c>
-      <c r="M2" s="1">
+      <c r="N2" s="1">
         <v>0.97325247228009426</v>
       </c>
-      <c r="N2" s="1">
+      <c r="O2" s="1">
         <v>0.14264121946353248</v>
       </c>
-      <c r="O2" s="1">
+      <c r="P2" s="1">
         <v>0.36217680575602773</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>45000</v>
+      </c>
+      <c r="B3" s="1">
         <v>0.31063492316583607</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C3" s="1">
         <v>0.30071206799015238</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>8.7881863818940475E-2</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>7.1104701442271656E-3</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>0.30364383047323162</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>0.51535238422054863</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>0.68588790425543422</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>0.74208499777642267</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>0.25451197854658725</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>0.71422181445359789</v>
       </c>
-      <c r="K3" s="1">
+      <c r="L3" s="1">
         <v>0.76247377079320611</v>
       </c>
-      <c r="L3" s="1">
+      <c r="M3" s="1">
         <v>0.35210985554934493</v>
       </c>
-      <c r="M3" s="1">
+      <c r="N3" s="1">
         <v>0.30832742958856008</v>
       </c>
-      <c r="N3" s="1">
+      <c r="O3" s="1">
         <v>0.11969879576137277</v>
       </c>
-      <c r="O3" s="1">
+      <c r="P3" s="1">
         <v>0.57049306713871795</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>44999</v>
+      </c>
+      <c r="B4" s="1">
         <v>0.13344244634761715</v>
       </c>
-      <c r="B4" s="1">
+      <c r="C4" s="1">
         <v>6.989083663714668E-2</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>0.44502464131542341</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>0.35399525448379821</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>0.53788539984121586</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>0.47609383327654531</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>0.55139084881206579</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>0.69538527350025603</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <v>0.48393583678744223</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <v>0.5606687948103185</v>
       </c>
-      <c r="K4" s="1">
+      <c r="L4" s="1">
         <v>0.83262871452785325</v>
       </c>
-      <c r="L4" s="1">
+      <c r="M4" s="1">
         <v>0.33765900128434712</v>
       </c>
-      <c r="M4" s="1">
+      <c r="N4" s="1">
         <v>0.84514981483155327</v>
       </c>
-      <c r="N4" s="1">
+      <c r="O4" s="1">
         <v>0.41287899472258349</v>
       </c>
-      <c r="O4" s="1">
+      <c r="P4" s="1">
         <v>0.49178278516720386</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>44998</v>
+      </c>
+      <c r="B5" s="1">
         <v>0.44695395693861539</v>
       </c>
-      <c r="B5" s="1">
+      <c r="C5" s="1">
         <v>0.82985410120635272</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>0.56132197390295957</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>0.94207120102023512</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>0.26167965362901213</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>0.39804795937084103</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>0.77823044098119465</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>0.8397785741317616</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>0.21045529081866288</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>0.24989074666942335</v>
       </c>
-      <c r="K5" s="1">
+      <c r="L5" s="1">
         <v>0.34835229537484946</v>
       </c>
-      <c r="L5" s="1">
+      <c r="M5" s="1">
         <v>3.1078384884576482E-2</v>
       </c>
-      <c r="M5" s="1">
+      <c r="N5" s="1">
         <v>0.10118631472074568</v>
       </c>
-      <c r="N5" s="1">
+      <c r="O5" s="1">
         <v>0.10152040783994398</v>
       </c>
-      <c r="O5" s="1">
+      <c r="P5" s="1">
         <v>0.88109843707224844</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>44997</v>
+      </c>
+      <c r="B6" s="1">
         <v>0.79199020159072331</v>
       </c>
-      <c r="B6" s="1">
+      <c r="C6" s="1">
         <v>0.87225554078141831</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>3.5308825359822937E-2</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>0.54442523276908394</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>8.3922254947013553E-2</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>0.89375517235661939</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>0.4679105173467466</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>0.31587069545757818</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <v>0.52337445878632172</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K6" s="1">
         <v>0.85937894084155075</v>
       </c>
-      <c r="K6" s="1">
+      <c r="L6" s="1">
         <v>0.11515931092041332</v>
       </c>
-      <c r="L6" s="1">
+      <c r="M6" s="1">
         <v>0.70253034730879993</v>
       </c>
-      <c r="M6" s="1">
+      <c r="N6" s="1">
         <v>0.62039271171769339</v>
       </c>
-      <c r="N6" s="1">
+      <c r="O6" s="1">
         <v>0.88699378848462773</v>
       </c>
-      <c r="O6" s="1">
+      <c r="P6" s="1">
         <v>0.46410669824027495</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>44996</v>
+      </c>
+      <c r="B7" s="1">
         <v>0.62302095535992286</v>
       </c>
-      <c r="B7" s="1">
+      <c r="C7" s="1">
         <v>0.92077728583695273</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>0.17838503928094962</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>0.42976761303974609</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>0.71967205749303009</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>0.55005587056476246</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>0.35958748409919483</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>0.99953613447344591</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>0.40328674941751308</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K7" s="1">
         <v>0.94739700044822361</v>
       </c>
-      <c r="K7" s="1">
+      <c r="L7" s="1">
         <v>0.15330527347814649</v>
       </c>
-      <c r="L7" s="1">
+      <c r="M7" s="1">
         <v>0.73292387952654525</v>
       </c>
-      <c r="M7" s="1">
+      <c r="N7" s="1">
         <v>9.4036692586947468E-2</v>
       </c>
-      <c r="N7" s="1">
+      <c r="O7" s="1">
         <v>0.12713986636249008</v>
       </c>
-      <c r="O7" s="1">
+      <c r="P7" s="1">
         <v>0.78493366788635177</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>44995</v>
+      </c>
+      <c r="B8" s="1">
         <v>0.74812770767706649</v>
       </c>
-      <c r="B8" s="1">
+      <c r="C8" s="1">
         <v>0.96376169285360125</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>0.92767870435675071</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>0.70362240491339845</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>0.89515840075579511</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>0.48850549324436765</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <v>0.60722375355485658</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>0.42286815350424345</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8" s="1">
         <v>9.153935663658086E-2</v>
       </c>
-      <c r="J8" s="1">
+      <c r="K8" s="1">
         <v>0.82766099648162395</v>
       </c>
-      <c r="K8" s="1">
+      <c r="L8" s="1">
         <v>0.18317502695580168</v>
       </c>
-      <c r="L8" s="1">
+      <c r="M8" s="1">
         <v>0.1158784986985435</v>
       </c>
-      <c r="M8" s="1">
+      <c r="N8" s="1">
         <v>0.2591323318249843</v>
       </c>
-      <c r="N8" s="1">
+      <c r="O8" s="1">
         <v>0.89230727685328448</v>
       </c>
-      <c r="O8" s="1">
+      <c r="P8" s="1">
         <v>0.55435038901170874</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>44994</v>
+      </c>
+      <c r="B9" s="1">
         <v>0.53096647550450693</v>
       </c>
-      <c r="B9" s="1">
+      <c r="C9" s="1">
         <v>0.19487639510096155</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <v>0.72319113629519871</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>0.47916953896008341</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>0.67496458906576995</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9" s="1">
         <v>0.32204958404113393</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H9" s="1">
         <v>4.174660510471695E-2</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>0.61754840375456266</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J9" s="1">
         <v>0.96010366209188902</v>
       </c>
-      <c r="J9" s="1">
+      <c r="K9" s="1">
         <v>0.19121536144088991</v>
       </c>
-      <c r="K9" s="1">
+      <c r="L9" s="1">
         <v>0.21656114261588466</v>
       </c>
-      <c r="L9" s="1">
+      <c r="M9" s="1">
         <v>0.30302889542761635</v>
       </c>
-      <c r="M9" s="1">
+      <c r="N9" s="1">
         <v>0.71155790808154784</v>
       </c>
-      <c r="N9" s="1">
+      <c r="O9" s="1">
         <v>0.3974902037722905</v>
       </c>
-      <c r="O9" s="1">
+      <c r="P9" s="1">
         <v>0.6943237312057472</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>44993</v>
+      </c>
+      <c r="B10" s="1">
         <v>1.7064049463941355E-2</v>
       </c>
-      <c r="B10" s="1">
+      <c r="C10" s="1">
         <v>0.21527290722300385</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <v>4.2920710331012746E-2</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>0.58611086894116238</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>0.81224748445784578</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G10" s="1">
         <v>0.42482313556936679</v>
       </c>
-      <c r="G10" s="1">
+      <c r="H10" s="1">
         <v>0.71415614154622942</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>0.68868518968889814</v>
       </c>
-      <c r="I10" s="1">
+      <c r="J10" s="1">
         <v>0.74980655538290575</v>
       </c>
-      <c r="J10" s="1">
+      <c r="K10" s="1">
         <v>0.73694781906109375</v>
       </c>
-      <c r="K10" s="1">
+      <c r="L10" s="1">
         <v>0.90434414829205645</v>
       </c>
-      <c r="L10" s="1">
+      <c r="M10" s="1">
         <v>0.15634999809299588</v>
       </c>
-      <c r="M10" s="1">
+      <c r="N10" s="1">
         <v>0.93471326701749269</v>
       </c>
-      <c r="N10" s="1">
+      <c r="O10" s="1">
         <v>0.52551380620366261</v>
       </c>
-      <c r="O10" s="1">
+      <c r="P10" s="1">
         <v>3.8101864129233776E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>44992</v>
+      </c>
+      <c r="B11" s="1">
         <v>0.44987948525524346</v>
       </c>
-      <c r="B11" s="1">
+      <c r="C11" s="1">
         <v>0.90186766281684416</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>0.3483226454357915</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>0.48105581032634614</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>0.13563401625144722</v>
       </c>
-      <c r="F11" s="1">
+      <c r="G11" s="1">
         <v>0.2295737769166466</v>
       </c>
-      <c r="G11" s="1">
+      <c r="H11" s="1">
         <v>0.47436445041591624</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>0.85974652731959267</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J11" s="1">
         <v>0.29806952857452551</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K11" s="1">
         <v>0.8021903646864722</v>
       </c>
-      <c r="K11" s="1">
+      <c r="L11" s="1">
         <v>0.71027763169586611</v>
       </c>
-      <c r="L11" s="1">
+      <c r="M11" s="1">
         <v>0.35324918581848386</v>
       </c>
-      <c r="M11" s="1">
+      <c r="N11" s="1">
         <v>0.50354693380585624</v>
       </c>
-      <c r="N11" s="1">
+      <c r="O11" s="1">
         <v>0.12197313902774154</v>
       </c>
-      <c r="O11" s="1">
+      <c r="P11" s="1">
         <v>0.65411991719841267</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>44991</v>
+      </c>
+      <c r="B12" s="1">
         <v>0.78010012480811863</v>
       </c>
-      <c r="B12" s="1">
+      <c r="C12" s="1">
         <v>6.2837214931117935E-2</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <v>0.80930353225581253</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>0.83857014644939476</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
         <v>0.86063081693400134</v>
       </c>
-      <c r="F12" s="1">
+      <c r="G12" s="1">
         <v>0.56579175493688327</v>
       </c>
-      <c r="G12" s="1">
+      <c r="H12" s="1">
         <v>3.5074868715479934E-2</v>
       </c>
-      <c r="H12" s="1">
+      <c r="I12" s="1">
         <v>0.28492694438462873</v>
       </c>
-      <c r="I12" s="1">
+      <c r="J12" s="1">
         <v>0.13531379372562669</v>
       </c>
-      <c r="J12" s="1">
+      <c r="K12" s="1">
         <v>0.64841662861546245</v>
       </c>
-      <c r="K12" s="1">
+      <c r="L12" s="1">
         <v>0.88757272666292042</v>
       </c>
-      <c r="L12" s="1">
+      <c r="M12" s="1">
         <v>0.94556794432551261</v>
       </c>
-      <c r="M12" s="1">
+      <c r="N12" s="1">
         <v>8.3401224227172999E-2</v>
       </c>
-      <c r="N12" s="1">
+      <c r="O12" s="1">
         <v>0.94769341123649786</v>
       </c>
-      <c r="O12" s="1">
+      <c r="P12" s="1">
         <v>0.31113331786836462</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>44990</v>
+      </c>
+      <c r="B13" s="1">
         <v>0.27471852351329318</v>
       </c>
-      <c r="B13" s="1">
+      <c r="C13" s="1">
         <v>0.36977214022997074</v>
       </c>
-      <c r="C13" s="1">
+      <c r="D13" s="1">
         <v>0.77534947291896139</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E13" s="1">
         <v>0.90107456343840475</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F13" s="1">
         <v>0.59232158256979894</v>
       </c>
-      <c r="F13" s="1">
+      <c r="G13" s="1">
         <v>0.62798866598784575</v>
       </c>
-      <c r="G13" s="1">
+      <c r="H13" s="1">
         <v>0.11258693078366555</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <v>0.35811443689019595</v>
       </c>
-      <c r="I13" s="1">
+      <c r="J13" s="1">
         <v>0.21233277720229304</v>
       </c>
-      <c r="J13" s="1">
+      <c r="K13" s="1">
         <v>0.57408185999182182</v>
       </c>
-      <c r="K13" s="1">
+      <c r="L13" s="1">
         <v>0.89723080706456149</v>
       </c>
-      <c r="L13" s="1">
+      <c r="M13" s="1">
         <v>3.0816098688487559E-3</v>
       </c>
-      <c r="M13" s="1">
+      <c r="N13" s="1">
         <v>0.7482585472239327</v>
       </c>
-      <c r="N13" s="1">
+      <c r="O13" s="1">
         <v>0.94970970194618398</v>
       </c>
-      <c r="O13" s="1">
+      <c r="P13" s="1">
         <v>0.4881573319281215</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>44989</v>
+      </c>
+      <c r="B14" s="1">
         <v>0.90157598851381204</v>
       </c>
-      <c r="B14" s="1">
+      <c r="C14" s="1">
         <v>0.47354757841939665</v>
       </c>
-      <c r="C14" s="1">
+      <c r="D14" s="1">
         <v>0.453936154709915</v>
       </c>
-      <c r="D14" s="1">
+      <c r="E14" s="1">
         <v>0.28579065632270784</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F14" s="1">
         <v>0.4809121629735017</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G14" s="1">
         <v>0.27445260456179787</v>
       </c>
-      <c r="G14" s="1">
+      <c r="H14" s="1">
         <v>0.73259933581118197</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <v>0.27169246423717763</v>
       </c>
-      <c r="I14" s="1">
+      <c r="J14" s="1">
         <v>0.83296913139388706</v>
       </c>
-      <c r="J14" s="1">
+      <c r="K14" s="1">
         <v>0.26598235058086117</v>
       </c>
-      <c r="K14" s="1">
+      <c r="L14" s="1">
         <v>0.55301681989495433</v>
       </c>
-      <c r="L14" s="1">
+      <c r="M14" s="1">
         <v>0.49344867096088607</v>
       </c>
-      <c r="M14" s="1">
+      <c r="N14" s="1">
         <v>0.97461414036185079</v>
       </c>
-      <c r="N14" s="1">
+      <c r="O14" s="1">
         <v>0.73597623308048588</v>
       </c>
-      <c r="O14" s="1">
+      <c r="P14" s="1">
         <v>0.49205478108672807</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>44988</v>
+      </c>
+      <c r="B15" s="1">
         <v>0.1172779743927258</v>
       </c>
-      <c r="B15" s="1">
+      <c r="C15" s="1">
         <v>0.15463342182518036</v>
       </c>
-      <c r="C15" s="1">
+      <c r="D15" s="1">
         <v>0.78858142610783954</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E15" s="1">
         <v>0.34960551647927796</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F15" s="1">
         <v>0.32090464957411213</v>
       </c>
-      <c r="F15" s="1">
+      <c r="G15" s="1">
         <v>0.99432365374749831</v>
       </c>
-      <c r="G15" s="1">
+      <c r="H15" s="1">
         <v>0.52253357360047437</v>
       </c>
-      <c r="H15" s="1">
+      <c r="I15" s="1">
         <v>0.4808593359789185</v>
       </c>
-      <c r="I15" s="1">
+      <c r="J15" s="1">
         <v>0.13523534654022273</v>
       </c>
-      <c r="J15" s="1">
+      <c r="K15" s="1">
         <v>0.49300391583266057</v>
       </c>
-      <c r="K15" s="1">
+      <c r="L15" s="1">
         <v>0.68071515358319468</v>
       </c>
-      <c r="L15" s="1">
+      <c r="M15" s="1">
         <v>0.61088715388823756</v>
       </c>
-      <c r="M15" s="1">
+      <c r="N15" s="1">
         <v>0.96909074078238644</v>
       </c>
-      <c r="N15" s="1">
+      <c r="O15" s="1">
         <v>0.90821611041427186</v>
       </c>
-      <c r="O15" s="1">
+      <c r="P15" s="1">
         <v>0.55594654175009717</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>44987</v>
+      </c>
+      <c r="B16" s="1">
         <v>0.44099757216042956</v>
       </c>
-      <c r="B16" s="1">
+      <c r="C16" s="1">
         <v>0.82756959205432057</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D16" s="1">
         <v>9.8470170362251586E-2</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E16" s="1">
         <v>0.70057076101305371</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F16" s="1">
         <v>0.98701404324537267</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G16" s="1">
         <v>5.6916206367226496E-2</v>
       </c>
-      <c r="G16" s="1">
+      <c r="H16" s="1">
         <v>0.53045421308850405</v>
       </c>
-      <c r="H16" s="1">
+      <c r="I16" s="1">
         <v>0.37316252864645649</v>
       </c>
-      <c r="I16" s="1">
+      <c r="J16" s="1">
         <v>0.45692140968134531</v>
       </c>
-      <c r="J16" s="1">
+      <c r="K16" s="1">
         <v>0.14223853585259338</v>
       </c>
-      <c r="K16" s="1">
+      <c r="L16" s="1">
         <v>0.3602759292195219</v>
       </c>
-      <c r="L16" s="1">
+      <c r="M16" s="1">
         <v>6.8490349229789249E-2</v>
       </c>
-      <c r="M16" s="1">
+      <c r="N16" s="1">
         <v>0.96053896688366169</v>
       </c>
-      <c r="N16" s="1">
+      <c r="O16" s="1">
         <v>0.57283201448315457</v>
       </c>
-      <c r="O16" s="1">
+      <c r="P16" s="1">
         <v>0.99906529577073444</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>44986</v>
+      </c>
+      <c r="B17" s="1">
         <v>0.42001346157160691</v>
       </c>
-      <c r="B17" s="1">
+      <c r="C17" s="1">
         <v>0.29368960492151963</v>
       </c>
-      <c r="C17" s="1">
+      <c r="D17" s="1">
         <v>0.3177204110362023</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E17" s="1">
         <v>0.77575945408649827</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17" s="1">
         <v>0.3529910451383228</v>
       </c>
-      <c r="F17" s="1">
+      <c r="G17" s="1">
         <v>0.34656819495345847</v>
       </c>
-      <c r="G17" s="1">
+      <c r="H17" s="1">
         <v>0.51916355160912875</v>
       </c>
-      <c r="H17" s="1">
+      <c r="I17" s="1">
         <v>0.3189627454123789</v>
       </c>
-      <c r="I17" s="1">
+      <c r="J17" s="1">
         <v>0.50962604985319415</v>
       </c>
-      <c r="J17" s="1">
+      <c r="K17" s="1">
         <v>0.99877519085511601</v>
       </c>
-      <c r="K17" s="1">
+      <c r="L17" s="1">
         <v>0.56405574793083346</v>
       </c>
-      <c r="L17" s="1">
+      <c r="M17" s="1">
         <v>0.71816220277327536</v>
       </c>
-      <c r="M17" s="1">
+      <c r="N17" s="1">
         <v>0.68930570232893795</v>
       </c>
-      <c r="N17" s="1">
+      <c r="O17" s="1">
         <v>0.17250042652658781</v>
       </c>
-      <c r="O17" s="1">
+      <c r="P17" s="1">
         <v>0.37318151703168767</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>44985</v>
+      </c>
+      <c r="B18" s="1">
         <v>0.40370315115101407</v>
       </c>
-      <c r="B18" s="1">
+      <c r="C18" s="1">
         <v>0.83338967859365609</v>
       </c>
-      <c r="C18" s="1">
+      <c r="D18" s="1">
         <v>0.81431620473470512</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <v>0.84473677752221066</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18" s="1">
         <v>0.5654495966139631</v>
       </c>
-      <c r="F18" s="1">
+      <c r="G18" s="1">
         <v>3.0453105062453023E-2</v>
       </c>
-      <c r="G18" s="1">
+      <c r="H18" s="1">
         <v>0.85493713145616956</v>
       </c>
-      <c r="H18" s="1">
+      <c r="I18" s="1">
         <v>0.73723492021606418</v>
       </c>
-      <c r="I18" s="1">
+      <c r="J18" s="1">
         <v>0.49662555298884925</v>
       </c>
-      <c r="J18" s="1">
+      <c r="K18" s="1">
         <v>0.53997575167160727</v>
       </c>
-      <c r="K18" s="1">
+      <c r="L18" s="1">
         <v>0.45047439755963326</v>
       </c>
-      <c r="L18" s="1">
+      <c r="M18" s="1">
         <v>6.7299043752880205E-2</v>
       </c>
-      <c r="M18" s="1">
+      <c r="N18" s="1">
         <v>0.84562267331121443</v>
       </c>
-      <c r="N18" s="1">
+      <c r="O18" s="1">
         <v>0.24337061695456985</v>
       </c>
-      <c r="O18" s="1">
+      <c r="P18" s="1">
         <v>0.32462222535960716</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>44984</v>
+      </c>
+      <c r="B19" s="1">
         <v>0.25235074297817217</v>
       </c>
-      <c r="B19" s="1">
+      <c r="C19" s="1">
         <v>0.13535946942008237</v>
       </c>
-      <c r="C19" s="1">
+      <c r="D19" s="1">
         <v>0.83535001920079432</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E19" s="1">
         <v>0.30533417505646954</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
         <v>0.83271916794168543</v>
       </c>
-      <c r="F19" s="1">
+      <c r="G19" s="1">
         <v>0.67756224831248424</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H19" s="1">
         <v>0.7262154344571411</v>
       </c>
-      <c r="H19" s="1">
+      <c r="I19" s="1">
         <v>0.79208188628813248</v>
       </c>
-      <c r="I19" s="1">
+      <c r="J19" s="1">
         <v>0.36642482910827623</v>
       </c>
-      <c r="J19" s="1">
+      <c r="K19" s="1">
         <v>0.5429933577504471</v>
       </c>
-      <c r="K19" s="1">
+      <c r="L19" s="1">
         <v>0.3177827288028543</v>
       </c>
-      <c r="L19" s="1">
+      <c r="M19" s="1">
         <v>0.65176152115602637</v>
       </c>
-      <c r="M19" s="1">
+      <c r="N19" s="1">
         <v>2.6642779110673032E-2</v>
       </c>
-      <c r="N19" s="1">
+      <c r="O19" s="1">
         <v>0.75626620812671619</v>
       </c>
-      <c r="O19" s="1">
+      <c r="P19" s="1">
         <v>0.97962706553091494</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>44983</v>
+      </c>
+      <c r="B20" s="1">
         <v>0.45518326855892666</v>
       </c>
-      <c r="B20" s="1">
+      <c r="C20" s="1">
         <v>2.5352317120105328E-3</v>
       </c>
-      <c r="C20" s="1">
+      <c r="D20" s="1">
         <v>0.34406996959959824</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20" s="1">
         <v>0.82800171917452525</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20" s="1">
         <v>0.49604850374217591</v>
       </c>
-      <c r="F20" s="1">
+      <c r="G20" s="1">
         <v>0.65340211527901848</v>
       </c>
-      <c r="G20" s="1">
+      <c r="H20" s="1">
         <v>0.31622261369035165</v>
       </c>
-      <c r="H20" s="1">
+      <c r="I20" s="1">
         <v>0.54641656073330114</v>
       </c>
-      <c r="I20" s="1">
+      <c r="J20" s="1">
         <v>0.14216633978514714</v>
       </c>
-      <c r="J20" s="1">
+      <c r="K20" s="1">
         <v>0.82817438881731353</v>
       </c>
-      <c r="K20" s="1">
+      <c r="L20" s="1">
         <v>0.88047022212641157</v>
       </c>
-      <c r="L20" s="1">
+      <c r="M20" s="1">
         <v>0.52442744353832027</v>
       </c>
-      <c r="M20" s="1">
+      <c r="N20" s="1">
         <v>5.6382573285784443E-2</v>
       </c>
-      <c r="N20" s="1">
+      <c r="O20" s="1">
         <v>0.89575545176115967</v>
       </c>
-      <c r="O20" s="1">
+      <c r="P20" s="1">
         <v>0.82592533458028949</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>44982</v>
+      </c>
+      <c r="B21" s="1">
         <v>0.19268895792745511</v>
       </c>
-      <c r="B21" s="1">
+      <c r="C21" s="1">
         <v>4.5372647096026397E-2</v>
       </c>
-      <c r="C21" s="1">
+      <c r="D21" s="1">
         <v>0.95831444919021036</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E21" s="1">
         <v>0.49483638403767649</v>
       </c>
-      <c r="E21" s="1">
+      <c r="F21" s="1">
         <v>0.36275298684199175</v>
       </c>
-      <c r="F21" s="1">
+      <c r="G21" s="1">
         <v>0.41688887663864149</v>
       </c>
-      <c r="G21" s="1">
+      <c r="H21" s="1">
         <v>0.69387772237522594</v>
       </c>
-      <c r="H21" s="1">
+      <c r="I21" s="1">
         <v>0.23190757736720324</v>
       </c>
-      <c r="I21" s="1">
+      <c r="J21" s="1">
         <v>0.48919843496833626</v>
       </c>
-      <c r="J21" s="1">
+      <c r="K21" s="1">
         <v>0.36360900914144079</v>
       </c>
-      <c r="K21" s="1">
+      <c r="L21" s="1">
         <v>0.55850249210000502</v>
       </c>
-      <c r="L21" s="1">
+      <c r="M21" s="1">
         <v>0.521981019796943</v>
       </c>
-      <c r="M21" s="1">
+      <c r="N21" s="1">
         <v>5.1263815211832098E-2</v>
       </c>
-      <c r="N21" s="1">
+      <c r="O21" s="1">
         <v>0.33546263928844988</v>
       </c>
-      <c r="O21" s="1">
+      <c r="P21" s="1">
         <v>0.81580424084572389</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>44981</v>
+      </c>
+      <c r="B22" s="1">
         <v>0.3550819790480676</v>
       </c>
-      <c r="B22" s="1">
+      <c r="C22" s="1">
         <v>0.22169881047140028</v>
       </c>
-      <c r="C22" s="1">
+      <c r="D22" s="1">
         <v>0.62879207121178815</v>
       </c>
-      <c r="D22" s="1">
+      <c r="E22" s="1">
         <v>0.83596016641884685</v>
       </c>
-      <c r="E22" s="1">
+      <c r="F22" s="1">
         <v>0.37708484085179539</v>
       </c>
-      <c r="F22" s="1">
+      <c r="G22" s="1">
         <v>0.83429320124782447</v>
       </c>
-      <c r="G22" s="1">
+      <c r="H22" s="1">
         <v>0.95149821750835839</v>
       </c>
-      <c r="H22" s="1">
+      <c r="I22" s="1">
         <v>4.6408327604448352E-2</v>
       </c>
-      <c r="I22" s="1">
+      <c r="J22" s="1">
         <v>0.70153951904424616</v>
       </c>
-      <c r="J22" s="1">
+      <c r="K22" s="1">
         <v>0.83977463002125996</v>
       </c>
-      <c r="K22" s="1">
+      <c r="L22" s="1">
         <v>0.3719964856714234</v>
       </c>
-      <c r="L22" s="1">
+      <c r="M22" s="1">
         <v>0.39644144093205347</v>
       </c>
-      <c r="M22" s="1">
+      <c r="N22" s="1">
         <v>0.12992203495582921</v>
       </c>
-      <c r="N22" s="1">
+      <c r="O22" s="1">
         <v>0.44300699479760475</v>
       </c>
-      <c r="O22" s="1">
+      <c r="P22" s="1">
         <v>0.55378166471381562</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>44980</v>
+      </c>
+      <c r="B23" s="1">
         <v>0.75872422596247879</v>
       </c>
-      <c r="B23" s="1">
+      <c r="C23" s="1">
         <v>0.13612095478128594</v>
       </c>
-      <c r="C23" s="1">
+      <c r="D23" s="1">
         <v>0.83420552061442077</v>
       </c>
-      <c r="D23" s="1">
+      <c r="E23" s="1">
         <v>0.17227750091757454</v>
       </c>
-      <c r="E23" s="1">
+      <c r="F23" s="1">
         <v>2.3475260275258703E-2</v>
       </c>
-      <c r="F23" s="1">
+      <c r="G23" s="1">
         <v>6.2787771931284264E-2</v>
       </c>
-      <c r="G23" s="1">
+      <c r="H23" s="1">
         <v>0.8283375256587252</v>
       </c>
-      <c r="H23" s="1">
+      <c r="I23" s="1">
         <v>8.5783559477526472E-2</v>
       </c>
-      <c r="I23" s="1">
+      <c r="J23" s="1">
         <v>0.56723868103784325</v>
       </c>
-      <c r="J23" s="1">
+      <c r="K23" s="1">
         <v>7.9750928036712687E-2</v>
       </c>
-      <c r="K23" s="1">
+      <c r="L23" s="1">
         <v>0.27007710912202709</v>
       </c>
-      <c r="L23" s="1">
+      <c r="M23" s="1">
         <v>0.42723631439563936</v>
       </c>
-      <c r="M23" s="1">
+      <c r="N23" s="1">
         <v>0.40978468588901173</v>
       </c>
-      <c r="N23" s="1">
+      <c r="O23" s="1">
         <v>0.75528014344769034</v>
       </c>
-      <c r="O23" s="1">
+      <c r="P23" s="1">
         <v>0.89905536943207909</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>44979</v>
+      </c>
+      <c r="B24" s="1">
         <v>0.7898030625721929</v>
       </c>
-      <c r="B24" s="1">
+      <c r="C24" s="1">
         <v>8.0286277529988292E-2</v>
       </c>
-      <c r="C24" s="1">
+      <c r="D24" s="1">
         <v>0.9404408917562187</v>
       </c>
-      <c r="D24" s="1">
+      <c r="E24" s="1">
         <v>0.82477245988710179</v>
       </c>
-      <c r="E24" s="1">
+      <c r="F24" s="1">
         <v>0.60177518503187966</v>
       </c>
-      <c r="F24" s="1">
+      <c r="G24" s="1">
         <v>0.9899719264161897</v>
       </c>
-      <c r="G24" s="1">
+      <c r="H24" s="1">
         <v>0.18523066800652876</v>
       </c>
-      <c r="H24" s="1">
+      <c r="I24" s="1">
         <v>0.20447024408091885</v>
       </c>
-      <c r="I24" s="1">
+      <c r="J24" s="1">
         <v>0.24316075178653962</v>
       </c>
-      <c r="J24" s="1">
+      <c r="K24" s="1">
         <v>0.39634941694401615</v>
       </c>
-      <c r="K24" s="1">
+      <c r="L24" s="1">
         <v>8.6431069012832928E-2</v>
       </c>
-      <c r="L24" s="1">
+      <c r="M24" s="1">
         <v>0.29298336919057621</v>
       </c>
-      <c r="M24" s="1">
+      <c r="N24" s="1">
         <v>0.17158730843031156</v>
       </c>
-      <c r="N24" s="1">
+      <c r="O24" s="1">
         <v>0.76799424501980551</v>
       </c>
-      <c r="O24" s="1">
+      <c r="P24" s="1">
         <v>0.36901337029501902</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>44978</v>
+      </c>
+      <c r="B25" s="1">
         <v>0.19255221357152985</v>
       </c>
-      <c r="B25" s="1">
+      <c r="C25" s="1">
         <v>0.15839404928478984</v>
       </c>
-      <c r="C25" s="1">
+      <c r="D25" s="1">
         <v>0.88237223713703683</v>
       </c>
-      <c r="D25" s="1">
+      <c r="E25" s="1">
         <v>0.87123797460111185</v>
       </c>
-      <c r="E25" s="1">
+      <c r="F25" s="1">
         <v>0.81556552732802479</v>
       </c>
-      <c r="F25" s="1">
+      <c r="G25" s="1">
         <v>0.18449138909542906</v>
       </c>
-      <c r="G25" s="1">
+      <c r="H25" s="1">
         <v>0.23819263468013407</v>
       </c>
-      <c r="H25" s="1">
+      <c r="I25" s="1">
         <v>0.48524848532960974</v>
       </c>
-      <c r="I25" s="1">
+      <c r="J25" s="1">
         <v>0.84268595140113489</v>
       </c>
-      <c r="J25" s="1">
+      <c r="K25" s="1">
         <v>0.31501061334981251</v>
       </c>
-      <c r="K25" s="1">
+      <c r="L25" s="1">
         <v>0.76168977075829847</v>
       </c>
-      <c r="L25" s="1">
+      <c r="M25" s="1">
         <v>0.83718863026787049</v>
       </c>
-      <c r="M25" s="1">
+      <c r="N25" s="1">
         <v>0.36048476430148912</v>
       </c>
-      <c r="N25" s="1">
+      <c r="O25" s="1">
         <v>0.92054525066298265</v>
       </c>
-      <c r="O25" s="1">
+      <c r="P25" s="1">
         <v>0.4030107634125305</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>44977</v>
+      </c>
+      <c r="B26" s="1">
         <v>0.19417564599111181</v>
       </c>
-      <c r="B26" s="1">
+      <c r="C26" s="1">
         <v>8.6140208687483399E-2</v>
       </c>
-      <c r="C26" s="1">
+      <c r="D26" s="1">
         <v>0.20681673847084325</v>
       </c>
-      <c r="D26" s="1">
+      <c r="E26" s="1">
         <v>0.59744418601431515</v>
       </c>
-      <c r="E26" s="1">
+      <c r="F26" s="1">
         <v>0.61268793207453232</v>
       </c>
-      <c r="F26" s="1">
+      <c r="G26" s="1">
         <v>0.14816877108616877</v>
       </c>
-      <c r="G26" s="1">
+      <c r="H26" s="1">
         <v>0.4138130767503948</v>
       </c>
-      <c r="H26" s="1">
+      <c r="I26" s="1">
         <v>0.12405799851126931</v>
       </c>
-      <c r="I26" s="1">
+      <c r="J26" s="1">
         <v>0.17918564642556523</v>
       </c>
-      <c r="J26" s="1">
+      <c r="K26" s="1">
         <v>0.39424734906783254</v>
       </c>
-      <c r="K26" s="1">
+      <c r="L26" s="1">
         <v>0.1600784581238065</v>
       </c>
-      <c r="L26" s="1">
+      <c r="M26" s="1">
         <v>0.63911212188060629</v>
       </c>
-      <c r="M26" s="1">
+      <c r="N26" s="1">
         <v>0.73008301011909693</v>
       </c>
-      <c r="N26" s="1">
+      <c r="O26" s="1">
         <v>0.72680441233930748</v>
       </c>
-      <c r="O26" s="1">
+      <c r="P26" s="1">
         <v>0.40798416277761285</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>44976</v>
+      </c>
+      <c r="B27" s="1">
         <v>0.72799441135816489</v>
       </c>
-      <c r="B27" s="1">
+      <c r="C27" s="1">
         <v>0.86880808031792001</v>
       </c>
-      <c r="C27" s="1">
+      <c r="D27" s="1">
         <v>0.35580735011690923</v>
       </c>
-      <c r="D27" s="1">
+      <c r="E27" s="1">
         <v>0.35378785253950895</v>
       </c>
-      <c r="E27" s="1">
+      <c r="F27" s="1">
         <v>0.7069693783191725</v>
       </c>
-      <c r="F27" s="1">
+      <c r="G27" s="1">
         <v>0.82079491165794172</v>
       </c>
-      <c r="G27" s="1">
+      <c r="H27" s="1">
         <v>0.81902578095139378</v>
       </c>
-      <c r="H27" s="1">
+      <c r="I27" s="1">
         <v>0.17178871744342583</v>
       </c>
-      <c r="I27" s="1">
+      <c r="J27" s="1">
         <v>0.50577396160782317</v>
       </c>
-      <c r="J27" s="1">
+      <c r="K27" s="1">
         <v>0.20090027354854745</v>
       </c>
-      <c r="K27" s="1">
+      <c r="L27" s="1">
         <v>0.62853780545403692</v>
       </c>
-      <c r="L27" s="1">
+      <c r="M27" s="1">
         <v>5.7479869838264697E-2</v>
       </c>
-      <c r="M27" s="1">
+      <c r="N27" s="1">
         <v>0.23216300686582669</v>
       </c>
-      <c r="N27" s="1">
+      <c r="O27" s="1">
         <v>0.1050810963779153</v>
       </c>
-      <c r="O27" s="1">
+      <c r="P27" s="1">
         <v>0.64731119206760379</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>44975</v>
+      </c>
+      <c r="B28" s="1">
         <v>0.99739074092424074</v>
       </c>
-      <c r="B28" s="1">
+      <c r="C28" s="1">
         <v>0.21024883415265139</v>
       </c>
-      <c r="C28" s="1">
+      <c r="D28" s="1">
         <v>0.79657876816309769</v>
       </c>
-      <c r="D28" s="1">
+      <c r="E28" s="1">
         <v>5.4456815547597293E-2</v>
       </c>
-      <c r="E28" s="1">
+      <c r="F28" s="1">
         <v>5.4570207627055223E-2</v>
       </c>
-      <c r="F28" s="1">
+      <c r="G28" s="1">
         <v>0.93708560402317642</v>
       </c>
-      <c r="G28" s="1">
+      <c r="H28" s="1">
         <v>0.8317521614093969</v>
       </c>
-      <c r="H28" s="1">
+      <c r="I28" s="1">
         <v>0.37375074265842889</v>
       </c>
-      <c r="I28" s="1">
+      <c r="J28" s="1">
         <v>0.98300571664458236</v>
       </c>
-      <c r="J28" s="1">
+      <c r="K28" s="1">
         <v>0.44603166890723989</v>
       </c>
-      <c r="K28" s="1">
+      <c r="L28" s="1">
         <v>0.12902720359006703</v>
       </c>
-      <c r="L28" s="1">
+      <c r="M28" s="1">
         <v>9.345954655580857E-2</v>
       </c>
-      <c r="M28" s="1">
+      <c r="N28" s="1">
         <v>0.57399804277877509</v>
       </c>
-      <c r="N28" s="1">
+      <c r="O28" s="1">
         <v>0.10714351874638151</v>
       </c>
-      <c r="O28" s="1">
+      <c r="P28" s="1">
         <v>0.92479046823648248</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>44974</v>
+      </c>
+      <c r="B29" s="1">
         <v>0.18604348884382516</v>
       </c>
-      <c r="B29" s="1">
+      <c r="C29" s="1">
         <v>0.86609691205277617</v>
       </c>
-      <c r="C29" s="1">
+      <c r="D29" s="1">
         <v>7.5823068502059998E-2</v>
       </c>
-      <c r="D29" s="1">
+      <c r="E29" s="1">
         <v>0.28898051916051515</v>
       </c>
-      <c r="E29" s="1">
+      <c r="F29" s="1">
         <v>0.58048698430773693</v>
       </c>
-      <c r="F29" s="1">
+      <c r="G29" s="1">
         <v>0.33857163168216187</v>
       </c>
-      <c r="G29" s="1">
+      <c r="H29" s="1">
         <v>0.11378845352422562</v>
       </c>
-      <c r="H29" s="1">
+      <c r="I29" s="1">
         <v>0.73703373605201195</v>
       </c>
-      <c r="I29" s="1">
+      <c r="J29" s="1">
         <v>3.910443345013026E-2</v>
       </c>
-      <c r="J29" s="1">
+      <c r="K29" s="1">
         <v>0.68491342615819661</v>
       </c>
-      <c r="K29" s="1">
+      <c r="L29" s="1">
         <v>0.19508819743473427</v>
       </c>
-      <c r="L29" s="1">
+      <c r="M29" s="1">
         <v>0.80819739057602935</v>
       </c>
-      <c r="M29" s="1">
+      <c r="N29" s="1">
         <v>0.10098915517163998</v>
       </c>
-      <c r="N29" s="1">
+      <c r="O29" s="1">
         <v>0.5975290309501019</v>
       </c>
-      <c r="O29" s="1">
+      <c r="P29" s="1">
         <v>0.8667741391977053</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>44973</v>
+      </c>
+      <c r="B30" s="1">
         <v>0.76860480811276288</v>
       </c>
-      <c r="B30" s="1">
+      <c r="C30" s="1">
         <v>0.2298420318460308</v>
       </c>
-      <c r="C30" s="1">
+      <c r="D30" s="1">
         <v>0.3249754591559143</v>
       </c>
-      <c r="D30" s="1">
+      <c r="E30" s="1">
         <v>0.49787872622606133</v>
       </c>
-      <c r="E30" s="1">
+      <c r="F30" s="1">
         <v>0.9569627235483934</v>
       </c>
-      <c r="F30" s="1">
+      <c r="G30" s="1">
         <v>0.15421797240844359</v>
       </c>
-      <c r="G30" s="1">
+      <c r="H30" s="1">
         <v>0.75240306991615924</v>
       </c>
-      <c r="H30" s="1">
+      <c r="I30" s="1">
         <v>0.8991169356726626</v>
       </c>
-      <c r="I30" s="1">
+      <c r="J30" s="1">
         <v>0.17125858960938689</v>
       </c>
-      <c r="J30" s="1">
+      <c r="K30" s="1">
         <v>0.59067222364534144</v>
       </c>
-      <c r="K30" s="1">
+      <c r="L30" s="1">
         <v>0.46115977357965166</v>
       </c>
-      <c r="L30" s="1">
+      <c r="M30" s="1">
         <v>0.30686507620911951</v>
       </c>
-      <c r="M30" s="1">
+      <c r="N30" s="1">
         <v>0.60511289343536401</v>
       </c>
-      <c r="N30" s="1">
+      <c r="O30" s="1">
         <v>0.98314283347037135</v>
       </c>
-      <c r="O30" s="1">
+      <c r="P30" s="1">
         <v>0.54407654214788614</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>44972</v>
+      </c>
+      <c r="B31" s="1">
         <v>0.72566938926584057</v>
       </c>
-      <c r="B31" s="1">
+      <c r="C31" s="1">
         <v>0.39381863172049247</v>
       </c>
-      <c r="C31" s="1">
+      <c r="D31" s="1">
         <v>0.60763848591982095</v>
       </c>
-      <c r="D31" s="1">
+      <c r="E31" s="1">
         <v>0.93381059668685995</v>
       </c>
-      <c r="E31" s="1">
+      <c r="F31" s="1">
         <v>0.66492357869667451</v>
       </c>
-      <c r="F31" s="1">
+      <c r="G31" s="1">
         <v>0.94217059210623089</v>
       </c>
-      <c r="G31" s="1">
+      <c r="H31" s="1">
         <v>9.2691664630740855E-2</v>
       </c>
-      <c r="H31" s="1">
+      <c r="I31" s="1">
         <v>0.59704837094170804</v>
       </c>
-      <c r="I31" s="1">
+      <c r="J31" s="1">
         <v>0.56144778378142024</v>
       </c>
-      <c r="J31" s="1">
+      <c r="K31" s="1">
         <v>0.16007663427195484</v>
       </c>
-      <c r="K31" s="1">
+      <c r="L31" s="1">
         <v>0.15016556588523156</v>
       </c>
-      <c r="L31" s="1">
+      <c r="M31" s="1">
         <v>0.4583021103364997</v>
       </c>
-      <c r="M31" s="1">
+      <c r="N31" s="1">
         <v>0.45175076837749584</v>
       </c>
-      <c r="N31" s="1">
+      <c r="O31" s="1">
         <v>0.42464804928921973</v>
       </c>
-      <c r="O31" s="1">
+      <c r="P31" s="1">
         <v>0.53002566564121545</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <v>44971</v>
+      </c>
+      <c r="B32" s="1">
         <v>0.606844291381892</v>
       </c>
-      <c r="B32" s="1">
+      <c r="C32" s="1">
         <v>0.30095007997383671</v>
       </c>
-      <c r="C32" s="1">
+      <c r="D32" s="1">
         <v>0.2231948464985003</v>
       </c>
-      <c r="D32" s="1">
+      <c r="E32" s="1">
         <v>0.77299376205686199</v>
       </c>
-      <c r="E32" s="1">
+      <c r="F32" s="1">
         <v>0.74873235546488126</v>
       </c>
-      <c r="F32" s="1">
+      <c r="G32" s="1">
         <v>0.56524526960785237</v>
       </c>
-      <c r="G32" s="1">
+      <c r="H32" s="1">
         <v>0.10268747390497135</v>
       </c>
-      <c r="H32" s="1">
+      <c r="I32" s="1">
         <v>0.38537930771950646</v>
       </c>
-      <c r="I32" s="1">
+      <c r="J32" s="1">
         <v>0.55341241216786874</v>
       </c>
-      <c r="J32" s="1">
+      <c r="K32" s="1">
         <v>0.61235216992423458</v>
       </c>
-      <c r="K32" s="1">
+      <c r="L32" s="1">
         <v>0.78134324625797991</v>
       </c>
-      <c r="L32" s="1">
+      <c r="M32" s="1">
         <v>0.46152875903151824</v>
       </c>
-      <c r="M32" s="1">
+      <c r="N32" s="1">
         <v>0.17004289268953865</v>
       </c>
-      <c r="N32" s="1">
+      <c r="O32" s="1">
         <v>0.84731958088865345</v>
       </c>
-      <c r="O32" s="1">
+      <c r="P32" s="1">
         <v>0.83077837173618996</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <v>44970</v>
+      </c>
+      <c r="B33" s="1">
         <v>0.58923523043356618</v>
       </c>
-      <c r="B33" s="1">
+      <c r="C33" s="1">
         <v>0.90061701146394246</v>
       </c>
-      <c r="C33" s="1">
+      <c r="D33" s="1">
         <v>0.93897964689883218</v>
       </c>
-      <c r="D33" s="1">
+      <c r="E33" s="1">
         <v>0.78154120308672914</v>
       </c>
-      <c r="E33" s="1">
+      <c r="F33" s="1">
         <v>0.63191252269947229</v>
       </c>
-      <c r="F33" s="1">
+      <c r="G33" s="1">
         <v>0.41471625210827123</v>
       </c>
-      <c r="G33" s="1">
+      <c r="H33" s="1">
         <v>0.97025397582778028</v>
       </c>
-      <c r="H33" s="1">
+      <c r="I33" s="1">
         <v>0.7584879895298281</v>
       </c>
-      <c r="I33" s="1">
+      <c r="J33" s="1">
         <v>0.58603023986725555</v>
       </c>
-      <c r="J33" s="1">
+      <c r="K33" s="1">
         <v>0.40588085211762726</v>
       </c>
-      <c r="K33" s="1">
+      <c r="L33" s="1">
         <v>0.91872281170926373</v>
       </c>
-      <c r="L33" s="1">
+      <c r="M33" s="1">
         <v>0.86031166075389409</v>
       </c>
-      <c r="M33" s="1">
+      <c r="N33" s="1">
         <v>0.11705622781045188</v>
       </c>
-      <c r="N33" s="1">
+      <c r="O33" s="1">
         <v>0.46080556555102425</v>
       </c>
-      <c r="O33" s="1">
+      <c r="P33" s="1">
         <v>0.23412518328365217</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>44969</v>
+      </c>
+      <c r="B34" s="1">
         <v>0.15027189782946426</v>
       </c>
-      <c r="B34" s="1">
+      <c r="C34" s="1">
         <v>0.72628290748649316</v>
       </c>
-      <c r="C34" s="1">
+      <c r="D34" s="1">
         <v>0.30870161531989693</v>
       </c>
-      <c r="D34" s="1">
+      <c r="E34" s="1">
         <v>1.421013686925432E-2</v>
       </c>
-      <c r="E34" s="1">
+      <c r="F34" s="1">
         <v>0.63112117534204215</v>
       </c>
-      <c r="F34" s="1">
+      <c r="G34" s="1">
         <v>0.63994220418272407</v>
       </c>
-      <c r="G34" s="1">
+      <c r="H34" s="1">
         <v>0.24057374483419758</v>
       </c>
-      <c r="H34" s="1">
+      <c r="I34" s="1">
         <v>0.69429973267110368</v>
       </c>
-      <c r="I34" s="1">
+      <c r="J34" s="1">
         <v>0.48713407380436069</v>
       </c>
-      <c r="J34" s="1">
+      <c r="K34" s="1">
         <v>0.23232207153282924</v>
       </c>
-      <c r="K34" s="1">
+      <c r="L34" s="1">
         <v>0.90961418871717448</v>
       </c>
-      <c r="L34" s="1">
+      <c r="M34" s="1">
         <v>2.1378172360593917E-2</v>
       </c>
-      <c r="M34" s="1">
+      <c r="N34" s="1">
         <v>0.68307671105103884</v>
       </c>
-      <c r="N34" s="1">
+      <c r="O34" s="1">
         <v>0.30390971914647114</v>
       </c>
-      <c r="O34" s="1">
+      <c r="P34" s="1">
         <v>0.28214753647179647</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>44968</v>
+      </c>
+      <c r="B35" s="1">
         <v>4.021243186486112E-2</v>
       </c>
-      <c r="B35" s="1">
+      <c r="C35" s="1">
         <v>0.87122523666644969</v>
       </c>
-      <c r="C35" s="1">
+      <c r="D35" s="1">
         <v>0.52570810156725434</v>
       </c>
-      <c r="D35" s="1">
+      <c r="E35" s="1">
         <v>5.1775373820110993E-3</v>
       </c>
-      <c r="E35" s="1">
+      <c r="F35" s="1">
         <v>0.43057043101916237</v>
       </c>
-      <c r="F35" s="1">
+      <c r="G35" s="1">
         <v>0.72137241233098859</v>
       </c>
-      <c r="G35" s="1">
+      <c r="H35" s="1">
         <v>0.25769899005627084</v>
       </c>
-      <c r="H35" s="1">
+      <c r="I35" s="1">
         <v>0.64666424211089146</v>
       </c>
-      <c r="I35" s="1">
+      <c r="J35" s="1">
         <v>0.95029596484451306</v>
       </c>
-      <c r="J35" s="1">
+      <c r="K35" s="1">
         <v>1.8792648024394842E-2</v>
       </c>
-      <c r="K35" s="1">
+      <c r="L35" s="1">
         <v>0.80615970971784623</v>
       </c>
-      <c r="L35" s="1">
+      <c r="M35" s="1">
         <v>0.62974247074287426</v>
       </c>
-      <c r="M35" s="1">
+      <c r="N35" s="1">
         <v>0.67700872047271254</v>
       </c>
-      <c r="N35" s="1">
+      <c r="O35" s="1">
         <v>0.88321387379049532</v>
       </c>
-      <c r="O35" s="1">
+      <c r="P35" s="1">
         <v>4.2317083462770633E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>44967</v>
+      </c>
+      <c r="B36" s="1">
         <v>0.84903670607840087</v>
       </c>
-      <c r="B36" s="1">
+      <c r="C36" s="1">
         <v>0.22035950522441039</v>
       </c>
-      <c r="C36" s="1">
+      <c r="D36" s="1">
         <v>0.66492078679012279</v>
       </c>
-      <c r="D36" s="1">
+      <c r="E36" s="1">
         <v>0.85657088476168441</v>
       </c>
-      <c r="E36" s="1">
+      <c r="F36" s="1">
         <v>0.47061227308808617</v>
       </c>
-      <c r="F36" s="1">
+      <c r="G36" s="1">
         <v>0.38844729398926547</v>
       </c>
-      <c r="G36" s="1">
+      <c r="H36" s="1">
         <v>0.43035810601062618</v>
       </c>
-      <c r="H36" s="1">
+      <c r="I36" s="1">
         <v>0.70799394154236406</v>
       </c>
-      <c r="I36" s="1">
+      <c r="J36" s="1">
         <v>0.11429474197669387</v>
       </c>
-      <c r="J36" s="1">
+      <c r="K36" s="1">
         <v>0.82111887179761733</v>
       </c>
-      <c r="K36" s="1">
+      <c r="L36" s="1">
         <v>0.54512914939840285</v>
       </c>
-      <c r="L36" s="1">
+      <c r="M36" s="1">
         <v>0.44410417004063607</v>
       </c>
-      <c r="M36" s="1">
+      <c r="N36" s="1">
         <v>0.957751187882939</v>
       </c>
-      <c r="N36" s="1">
+      <c r="O36" s="1">
         <v>0.5214954980219445</v>
       </c>
-      <c r="O36" s="1">
+      <c r="P36" s="1">
         <v>0.90158423643708419</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>44966</v>
+      </c>
+      <c r="B37" s="1">
         <v>0.89266505923313044</v>
       </c>
-      <c r="B37" s="1">
+      <c r="C37" s="1">
         <v>0.80476775257267885</v>
       </c>
-      <c r="C37" s="1">
+      <c r="D37" s="1">
         <v>0.46884782061356978</v>
       </c>
-      <c r="D37" s="1">
+      <c r="E37" s="1">
         <v>0.72734911520794521</v>
       </c>
-      <c r="E37" s="1">
+      <c r="F37" s="1">
         <v>0.62747405041814786</v>
       </c>
-      <c r="F37" s="1">
+      <c r="G37" s="1">
         <v>0.62990872102998219</v>
       </c>
-      <c r="G37" s="1">
+      <c r="H37" s="1">
         <v>0.31257135093567023</v>
       </c>
-      <c r="H37" s="1">
+      <c r="I37" s="1">
         <v>0.40783538075306924</v>
       </c>
-      <c r="I37" s="1">
+      <c r="J37" s="1">
         <v>0.86744681602107321</v>
       </c>
-      <c r="J37" s="1">
+      <c r="K37" s="1">
         <v>0.71771437221763279</v>
       </c>
-      <c r="K37" s="1">
+      <c r="L37" s="1">
         <v>9.3475617742933004E-3</v>
       </c>
-      <c r="L37" s="1">
+      <c r="M37" s="1">
         <v>0.34615570242865246</v>
       </c>
-      <c r="M37" s="1">
+      <c r="N37" s="1">
         <v>0.63203695061291454</v>
       </c>
-      <c r="N37" s="1">
+      <c r="O37" s="1">
         <v>0.63684741088612162</v>
       </c>
-      <c r="O37" s="1">
+      <c r="P37" s="1">
         <v>7.2904847117551963E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>44965</v>
+      </c>
+      <c r="B38" s="1">
         <v>0.12037483343660138</v>
       </c>
-      <c r="B38" s="1">
+      <c r="C38" s="1">
         <v>2.3288552229641213E-2</v>
       </c>
-      <c r="C38" s="1">
+      <c r="D38" s="1">
         <v>1.4787179041257925E-2</v>
       </c>
-      <c r="D38" s="1">
+      <c r="E38" s="1">
         <v>0.96002591813339144</v>
       </c>
-      <c r="E38" s="1">
+      <c r="F38" s="1">
         <v>0.64624564363731107</v>
       </c>
-      <c r="F38" s="1">
+      <c r="G38" s="1">
         <v>0.84082586541752113</v>
       </c>
-      <c r="G38" s="1">
+      <c r="H38" s="1">
         <v>0.53515782023160874</v>
       </c>
-      <c r="H38" s="1">
+      <c r="I38" s="1">
         <v>0.27320841289041908</v>
       </c>
-      <c r="I38" s="1">
+      <c r="J38" s="1">
         <v>2.0368657965473491E-2</v>
       </c>
-      <c r="J38" s="1">
+      <c r="K38" s="1">
         <v>0.59253031657963573</v>
       </c>
-      <c r="K38" s="1">
+      <c r="L38" s="1">
         <v>0.15502362561300276</v>
       </c>
-      <c r="L38" s="1">
+      <c r="M38" s="1">
         <v>0.55172961693306366</v>
       </c>
-      <c r="M38" s="1">
+      <c r="N38" s="1">
         <v>0.6784064992247637</v>
       </c>
-      <c r="N38" s="1">
+      <c r="O38" s="1">
         <v>0.51694881219373745</v>
       </c>
-      <c r="O38" s="1">
+      <c r="P38" s="1">
         <v>0.95039261548020748</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <v>44964</v>
+      </c>
+      <c r="B39" s="1">
         <v>0.62993758451040993</v>
       </c>
-      <c r="B39" s="1">
+      <c r="C39" s="1">
         <v>0.77718067528036983</v>
       </c>
-      <c r="C39" s="1">
+      <c r="D39" s="1">
         <v>0.44775924138125711</v>
       </c>
-      <c r="D39" s="1">
+      <c r="E39" s="1">
         <v>0.69570773480837145</v>
       </c>
-      <c r="E39" s="1">
+      <c r="F39" s="1">
         <v>0.58140652097443246</v>
       </c>
-      <c r="F39" s="1">
+      <c r="G39" s="1">
         <v>0.21303681999292268</v>
       </c>
-      <c r="G39" s="1">
+      <c r="H39" s="1">
         <v>0.35271833238828365</v>
       </c>
-      <c r="H39" s="1">
+      <c r="I39" s="1">
         <v>2.7769056926193803E-2</v>
       </c>
-      <c r="I39" s="1">
+      <c r="J39" s="1">
         <v>0.63626749761656487</v>
       </c>
-      <c r="J39" s="1">
+      <c r="K39" s="1">
         <v>0.76485243326012631</v>
       </c>
-      <c r="K39" s="1">
+      <c r="L39" s="1">
         <v>6.9017963783692404E-2</v>
       </c>
-      <c r="L39" s="1">
+      <c r="M39" s="1">
         <v>0.80100607843528837</v>
       </c>
-      <c r="M39" s="1">
+      <c r="N39" s="1">
         <v>0.68048937358252226</v>
       </c>
-      <c r="N39" s="1">
+      <c r="O39" s="1">
         <v>0.58683920991395144</v>
       </c>
-      <c r="O39" s="1">
+      <c r="P39" s="1">
         <v>0.94361273614268881</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
+        <v>44963</v>
+      </c>
+      <c r="B40" s="1">
         <v>0.55532143239551923</v>
       </c>
-      <c r="B40" s="1">
+      <c r="C40" s="1">
         <v>0.14769013067093784</v>
       </c>
-      <c r="C40" s="1">
+      <c r="D40" s="1">
         <v>0.14863608861245359</v>
       </c>
-      <c r="D40" s="1">
+      <c r="E40" s="1">
         <v>0.93448163347746216</v>
       </c>
-      <c r="E40" s="1">
+      <c r="F40" s="1">
         <v>0.44154734584604194</v>
       </c>
-      <c r="F40" s="1">
+      <c r="G40" s="1">
         <v>0.88484617176975822</v>
       </c>
-      <c r="G40" s="1">
+      <c r="H40" s="1">
         <v>0.64795174412391676</v>
       </c>
-      <c r="H40" s="1">
+      <c r="I40" s="1">
         <v>0.72919916159694487</v>
       </c>
-      <c r="I40" s="1">
+      <c r="J40" s="1">
         <v>0.60435615881743865</v>
       </c>
-      <c r="J40" s="1">
+      <c r="K40" s="1">
         <v>0.16176969763620386</v>
       </c>
-      <c r="K40" s="1">
+      <c r="L40" s="1">
         <v>0.1413341466258462</v>
       </c>
-      <c r="L40" s="1">
+      <c r="M40" s="1">
         <v>0.40766744778329211</v>
       </c>
-      <c r="M40" s="1">
+      <c r="N40" s="1">
         <v>0.86715367763526285</v>
       </c>
-      <c r="N40" s="1">
+      <c r="O40" s="1">
         <v>0.36525079521309822</v>
       </c>
-      <c r="O40" s="1">
+      <c r="P40" s="1">
         <v>0.23273030119647142</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A41" s="1">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <v>44962</v>
+      </c>
+      <c r="B41" s="1">
         <v>7.4251543823143695E-2</v>
       </c>
-      <c r="B41" s="1">
+      <c r="C41" s="1">
         <v>0.37220583035418087</v>
       </c>
-      <c r="C41" s="1">
+      <c r="D41" s="1">
         <v>0.83433861770643469</v>
       </c>
-      <c r="D41" s="1">
+      <c r="E41" s="1">
         <v>6.2747460319007131E-2</v>
       </c>
-      <c r="E41" s="1">
+      <c r="F41" s="1">
         <v>0.80979678483019568</v>
       </c>
-      <c r="F41" s="1">
+      <c r="G41" s="1">
         <v>2.8432939813672231E-2</v>
       </c>
-      <c r="G41" s="1">
+      <c r="H41" s="1">
         <v>0.40554547419887454</v>
       </c>
-      <c r="H41" s="1">
+      <c r="I41" s="1">
         <v>0.40828091471655292</v>
       </c>
-      <c r="I41" s="1">
+      <c r="J41" s="1">
         <v>0.83803925855379502</v>
       </c>
-      <c r="J41" s="1">
+      <c r="K41" s="1">
         <v>0.92326396495168372</v>
       </c>
-      <c r="K41" s="1">
+      <c r="L41" s="1">
         <v>0.57351973124191358</v>
       </c>
-      <c r="L41" s="1">
+      <c r="M41" s="1">
         <v>0.30503793412412827</v>
       </c>
-      <c r="M41" s="1">
+      <c r="N41" s="1">
         <v>0.91864153419758576</v>
       </c>
-      <c r="N41" s="1">
+      <c r="O41" s="1">
         <v>0.85000347854588887</v>
       </c>
-      <c r="O41" s="1">
+      <c r="P41" s="1">
         <v>0.72071670858820813</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A42" s="1">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
+        <v>44961</v>
+      </c>
+      <c r="B42" s="1">
         <v>0.350144440216832</v>
       </c>
-      <c r="B42" s="1">
+      <c r="C42" s="1">
         <v>0.56993659532794771</v>
       </c>
-      <c r="C42" s="1">
+      <c r="D42" s="1">
         <v>0.71948867521538329</v>
       </c>
-      <c r="D42" s="1">
+      <c r="E42" s="1">
         <v>0.17978785038196221</v>
       </c>
-      <c r="E42" s="1">
+      <c r="F42" s="1">
         <v>0.9958721922721766</v>
       </c>
-      <c r="F42" s="1">
+      <c r="G42" s="1">
         <v>0.11865547314705238</v>
       </c>
-      <c r="G42" s="1">
+      <c r="H42" s="1">
         <v>0.77351293881658645</v>
       </c>
-      <c r="H42" s="1">
+      <c r="I42" s="1">
         <v>0.96296549391896369</v>
       </c>
-      <c r="I42" s="1">
+      <c r="J42" s="1">
         <v>0.69168837971789943</v>
       </c>
-      <c r="J42" s="1">
+      <c r="K42" s="1">
         <v>8.4017659420126067E-2</v>
       </c>
-      <c r="K42" s="1">
+      <c r="L42" s="1">
         <v>0.7883283627911698</v>
       </c>
-      <c r="L42" s="1">
+      <c r="M42" s="1">
         <v>0.13302637515920457</v>
       </c>
-      <c r="M42" s="1">
+      <c r="N42" s="1">
         <v>0.75217330158656814</v>
       </c>
-      <c r="N42" s="1">
+      <c r="O42" s="1">
         <v>0.84398380130173012</v>
       </c>
-      <c r="O42" s="1">
+      <c r="P42" s="1">
         <v>8.3908711646410339E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A43" s="1">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
+        <v>44960</v>
+      </c>
+      <c r="B43" s="1">
         <v>0.75789873238482608</v>
       </c>
-      <c r="B43" s="1">
+      <c r="C43" s="1">
         <v>0.33038201277628731</v>
       </c>
-      <c r="C43" s="1">
+      <c r="D43" s="1">
         <v>0.710657869785844</v>
       </c>
-      <c r="D43" s="1">
+      <c r="E43" s="1">
         <v>0.46664992582822351</v>
       </c>
-      <c r="E43" s="1">
+      <c r="F43" s="1">
         <v>9.7294207069263505E-2</v>
       </c>
-      <c r="F43" s="1">
+      <c r="G43" s="1">
         <v>0.69566890041979423</v>
       </c>
-      <c r="G43" s="1">
+      <c r="H43" s="1">
         <v>0.72779059398184487</v>
       </c>
-      <c r="H43" s="1">
+      <c r="I43" s="1">
         <v>0.69272493946897129</v>
       </c>
-      <c r="I43" s="1">
+      <c r="J43" s="1">
         <v>0.32614616880187208</v>
       </c>
-      <c r="J43" s="1">
+      <c r="K43" s="1">
         <v>0.69643143098636917</v>
       </c>
-      <c r="K43" s="1">
+      <c r="L43" s="1">
         <v>0.41933267266865182</v>
       </c>
-      <c r="L43" s="1">
+      <c r="M43" s="1">
         <v>0.28567346938982952</v>
       </c>
-      <c r="M43" s="1">
+      <c r="N43" s="1">
         <v>0.22390964641202593</v>
       </c>
-      <c r="N43" s="1">
+      <c r="O43" s="1">
         <v>0.91714084357756243</v>
       </c>
-      <c r="O43" s="1">
+      <c r="P43" s="1">
         <v>0.92016093354423267</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A44" s="1">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
+        <v>44959</v>
+      </c>
+      <c r="B44" s="1">
         <v>0.20337417636893074</v>
       </c>
-      <c r="B44" s="1">
+      <c r="C44" s="1">
         <v>0.83139221385661155</v>
       </c>
-      <c r="C44" s="1">
+      <c r="D44" s="1">
         <v>0.58211971273634289</v>
       </c>
-      <c r="D44" s="1">
+      <c r="E44" s="1">
         <v>4.3084808625976856E-2</v>
       </c>
-      <c r="E44" s="1">
+      <c r="F44" s="1">
         <v>0.22693068865027644</v>
       </c>
-      <c r="F44" s="1">
+      <c r="G44" s="1">
         <v>0.11176413656108275</v>
       </c>
-      <c r="G44" s="1">
+      <c r="H44" s="1">
         <v>0.59550518868684654</v>
       </c>
-      <c r="H44" s="1">
+      <c r="I44" s="1">
         <v>0.15930035540661114</v>
       </c>
-      <c r="I44" s="1">
+      <c r="J44" s="1">
         <v>0.88722703390730528</v>
       </c>
-      <c r="J44" s="1">
+      <c r="K44" s="1">
         <v>0.86453670699260843</v>
       </c>
-      <c r="K44" s="1">
+      <c r="L44" s="1">
         <v>0.47711845984052137</v>
       </c>
-      <c r="L44" s="1">
+      <c r="M44" s="1">
         <v>9.9077129992074631E-2</v>
       </c>
-      <c r="M44" s="1">
+      <c r="N44" s="1">
         <v>6.0732622499628297E-2</v>
       </c>
-      <c r="N44" s="1">
+      <c r="O44" s="1">
         <v>0.25188681243364475</v>
       </c>
-      <c r="O44" s="1">
+      <c r="P44" s="1">
         <v>0.21785491276273383</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A45" s="1">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
+        <v>44958</v>
+      </c>
+      <c r="B45" s="1">
         <v>0.31420820725224774</v>
       </c>
-      <c r="B45" s="1">
+      <c r="C45" s="1">
         <v>0.4866165490026706</v>
       </c>
-      <c r="C45" s="1">
+      <c r="D45" s="1">
         <v>0.65191039741648016</v>
       </c>
-      <c r="D45" s="1">
+      <c r="E45" s="1">
         <v>1.1876724116649306E-2</v>
       </c>
-      <c r="E45" s="1">
+      <c r="F45" s="1">
         <v>0.75599705583805821</v>
       </c>
-      <c r="F45" s="1">
+      <c r="G45" s="1">
         <v>0.18361546427853781</v>
       </c>
-      <c r="G45" s="1">
+      <c r="H45" s="1">
         <v>0.47254090461441978</v>
       </c>
-      <c r="H45" s="1">
+      <c r="I45" s="1">
         <v>0.47993198623330646</v>
       </c>
-      <c r="I45" s="1">
+      <c r="J45" s="1">
         <v>0.77382343034208678</v>
       </c>
-      <c r="J45" s="1">
+      <c r="K45" s="1">
         <v>0.59339616121372651</v>
       </c>
-      <c r="K45" s="1">
+      <c r="L45" s="1">
         <v>0.40059329230453899</v>
       </c>
-      <c r="L45" s="1">
+      <c r="M45" s="1">
         <v>8.431084059207139E-2</v>
       </c>
-      <c r="M45" s="1">
+      <c r="N45" s="1">
         <v>0.81838110686627996</v>
       </c>
-      <c r="N45" s="1">
+      <c r="O45" s="1">
         <v>0.38191676503728544</v>
       </c>
-      <c r="O45" s="1">
+      <c r="P45" s="1">
         <v>1.0580427121977265E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A46" s="1">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
+        <v>44957</v>
+      </c>
+      <c r="B46" s="1">
         <v>0.87705507782162828</v>
       </c>
-      <c r="B46" s="1">
+      <c r="C46" s="1">
         <v>0.52368635085045268</v>
       </c>
-      <c r="C46" s="1">
+      <c r="D46" s="1">
         <v>0.98428650205228785</v>
       </c>
-      <c r="D46" s="1">
+      <c r="E46" s="1">
         <v>0.99633162536826836</v>
       </c>
-      <c r="E46" s="1">
+      <c r="F46" s="1">
         <v>0.91537362047168003</v>
       </c>
-      <c r="F46" s="1">
+      <c r="G46" s="1">
         <v>0.32468419334811716</v>
       </c>
-      <c r="G46" s="1">
+      <c r="H46" s="1">
         <v>0.82464783365198013</v>
       </c>
-      <c r="H46" s="1">
+      <c r="I46" s="1">
         <v>6.313385127120108E-2</v>
       </c>
-      <c r="I46" s="1">
+      <c r="J46" s="1">
         <v>0.75174836944559287</v>
       </c>
-      <c r="J46" s="1">
+      <c r="K46" s="1">
         <v>0.54965134639018653</v>
       </c>
-      <c r="K46" s="1">
+      <c r="L46" s="1">
         <v>0.82950241663102853</v>
       </c>
-      <c r="L46" s="1">
+      <c r="M46" s="1">
         <v>0.62244171278977733</v>
       </c>
-      <c r="M46" s="1">
+      <c r="N46" s="1">
         <v>0.42491540627909052</v>
       </c>
-      <c r="N46" s="1">
+      <c r="O46" s="1">
         <v>0.24639026417627741</v>
       </c>
-      <c r="O46" s="1">
+      <c r="P46" s="1">
         <v>0.34504441797405083</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A47" s="1">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
+        <v>44956</v>
+      </c>
+      <c r="B47" s="1">
         <v>4.0675021055822436E-2</v>
       </c>
-      <c r="B47" s="1">
+      <c r="C47" s="1">
         <v>0.86382798324349952</v>
       </c>
-      <c r="C47" s="1">
+      <c r="D47" s="1">
         <v>0.1176122803768862</v>
       </c>
-      <c r="D47" s="1">
+      <c r="E47" s="1">
         <v>0.59272773048228833</v>
       </c>
-      <c r="E47" s="1">
+      <c r="F47" s="1">
         <v>0.57648942250477098</v>
       </c>
-      <c r="F47" s="1">
+      <c r="G47" s="1">
         <v>7.5598373792303608E-2</v>
       </c>
-      <c r="G47" s="1">
+      <c r="H47" s="1">
         <v>0.8559237440373193</v>
       </c>
-      <c r="H47" s="1">
+      <c r="I47" s="1">
         <v>0.26259075659027642</v>
       </c>
-      <c r="I47" s="1">
+      <c r="J47" s="1">
         <v>0.51813851658149035</v>
       </c>
-      <c r="J47" s="1">
+      <c r="K47" s="1">
         <v>0.49320604017799208</v>
       </c>
-      <c r="K47" s="1">
+      <c r="L47" s="1">
         <v>0.73794293807969513</v>
       </c>
-      <c r="L47" s="1">
+      <c r="M47" s="1">
         <v>0.32187020039208958</v>
       </c>
-      <c r="M47" s="1">
+      <c r="N47" s="1">
         <v>0.5405093326526641</v>
       </c>
-      <c r="N47" s="1">
+      <c r="O47" s="1">
         <v>0.81792461450753884</v>
       </c>
-      <c r="O47" s="1">
+      <c r="P47" s="1">
         <v>0.2879997218638064</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A48" s="1">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
+        <v>44955</v>
+      </c>
+      <c r="B48" s="1">
         <v>0.28605742142627932</v>
       </c>
-      <c r="B48" s="1">
+      <c r="C48" s="1">
         <v>0.22296575287346054</v>
       </c>
-      <c r="C48" s="1">
+      <c r="D48" s="1">
         <v>0.46279592671977665</v>
       </c>
-      <c r="D48" s="1">
+      <c r="E48" s="1">
         <v>0.71915980803236845</v>
       </c>
-      <c r="E48" s="1">
+      <c r="F48" s="1">
         <v>0.11187906478191323</v>
       </c>
-      <c r="F48" s="1">
+      <c r="G48" s="1">
         <v>0.77882793444163245</v>
       </c>
-      <c r="G48" s="1">
+      <c r="H48" s="1">
         <v>0.6329086106463786</v>
       </c>
-      <c r="H48" s="1">
+      <c r="I48" s="1">
         <v>0.20517783330552486</v>
       </c>
-      <c r="I48" s="1">
+      <c r="J48" s="1">
         <v>0.75568991150850084</v>
       </c>
-      <c r="J48" s="1">
+      <c r="K48" s="1">
         <v>0.49811247303282569</v>
       </c>
-      <c r="K48" s="1">
+      <c r="L48" s="1">
         <v>0.84968736251408705</v>
       </c>
-      <c r="L48" s="1">
+      <c r="M48" s="1">
         <v>0.7393923860687831</v>
       </c>
-      <c r="M48" s="1">
+      <c r="N48" s="1">
         <v>0.63556449313252306</v>
       </c>
-      <c r="N48" s="1">
+      <c r="O48" s="1">
         <v>0.27368335952400002</v>
       </c>
-      <c r="O48" s="1">
+      <c r="P48" s="1">
         <v>4.0224557191256394E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A49" s="1">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A49" s="2">
+        <v>44954</v>
+      </c>
+      <c r="B49" s="1">
         <v>0.48961228807125379</v>
       </c>
-      <c r="B49" s="1">
+      <c r="C49" s="1">
         <v>1.1141520970072483E-2</v>
       </c>
-      <c r="C49" s="1">
+      <c r="D49" s="1">
         <v>0.73849495994108161</v>
       </c>
-      <c r="D49" s="1">
+      <c r="E49" s="1">
         <v>0.94492590170698687</v>
       </c>
-      <c r="E49" s="1">
+      <c r="F49" s="1">
         <v>0.27270580958221236</v>
       </c>
-      <c r="F49" s="1">
+      <c r="G49" s="1">
         <v>0.97307674352562201</v>
       </c>
-      <c r="G49" s="1">
+      <c r="H49" s="1">
         <v>0.25518107314731708</v>
       </c>
-      <c r="H49" s="1">
+      <c r="I49" s="1">
         <v>0.68071959245123759</v>
       </c>
-      <c r="I49" s="1">
+      <c r="J49" s="1">
         <v>0.17647077702526837</v>
       </c>
-      <c r="J49" s="1">
+      <c r="K49" s="1">
         <v>0.42167829759610598</v>
       </c>
-      <c r="K49" s="1">
+      <c r="L49" s="1">
         <v>0.25715938781997671</v>
       </c>
-      <c r="L49" s="1">
+      <c r="M49" s="1">
         <v>0.47308134953215486</v>
       </c>
-      <c r="M49" s="1">
+      <c r="N49" s="1">
         <v>0.85523195220909398</v>
       </c>
-      <c r="N49" s="1">
+      <c r="O49" s="1">
         <v>0.61547074481519837</v>
       </c>
-      <c r="O49" s="1">
+      <c r="P49" s="1">
         <v>4.0688811562836769E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A50" s="1">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A50" s="2">
+        <v>44953</v>
+      </c>
+      <c r="B50" s="1">
         <v>0.29217022296075468</v>
       </c>
-      <c r="B50" s="1">
+      <c r="C50" s="1">
         <v>0.79400690205847491</v>
       </c>
-      <c r="C50" s="1">
+      <c r="D50" s="1">
         <v>0.56135802134234347</v>
       </c>
-      <c r="D50" s="1">
+      <c r="E50" s="1">
         <v>0.46556173400162271</v>
       </c>
-      <c r="E50" s="1">
+      <c r="F50" s="1">
         <v>0.57565541944875587</v>
       </c>
-      <c r="F50" s="1">
+      <c r="G50" s="1">
         <v>0.33867959999889985</v>
       </c>
-      <c r="G50" s="1">
+      <c r="H50" s="1">
         <v>0.63442946477096041</v>
       </c>
-      <c r="H50" s="1">
+      <c r="I50" s="1">
         <v>0.58733392315537369</v>
       </c>
-      <c r="I50" s="1">
+      <c r="J50" s="1">
         <v>0.975729639291955</v>
       </c>
-      <c r="J50" s="1">
+      <c r="K50" s="1">
         <v>0.44107356615087634</v>
       </c>
-      <c r="K50" s="1">
+      <c r="L50" s="1">
         <v>0.40538399797713343</v>
       </c>
-      <c r="L50" s="1">
+      <c r="M50" s="1">
         <v>0.30930379739464497</v>
       </c>
-      <c r="M50" s="1">
+      <c r="N50" s="1">
         <v>0.80927928088257206</v>
       </c>
-      <c r="N50" s="1">
+      <c r="O50" s="1">
         <v>0.22990788895128522</v>
       </c>
-      <c r="O50" s="1">
+      <c r="P50" s="1">
         <v>0.12355258521125956</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A51" s="1">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A51" s="2">
+        <v>44952</v>
+      </c>
+      <c r="B51" s="1">
         <v>0.98229637482397369</v>
       </c>
-      <c r="B51" s="1">
+      <c r="C51" s="1">
         <v>0.21602192044039203</v>
       </c>
-      <c r="C51" s="1">
+      <c r="D51" s="1">
         <v>0.83292470474566593</v>
       </c>
-      <c r="D51" s="1">
+      <c r="E51" s="1">
         <v>0.61595914901080495</v>
       </c>
-      <c r="E51" s="1">
+      <c r="F51" s="1">
         <v>0.91254873699610817</v>
       </c>
-      <c r="F51" s="1">
+      <c r="G51" s="1">
         <v>8.8161061868054169E-2</v>
       </c>
-      <c r="G51" s="1">
+      <c r="H51" s="1">
         <v>0.71705336361689676</v>
       </c>
-      <c r="H51" s="1">
+      <c r="I51" s="1">
         <v>0.76039083470037971</v>
       </c>
-      <c r="I51" s="1">
+      <c r="J51" s="1">
         <v>0.61659886942974251</v>
       </c>
-      <c r="J51" s="1">
+      <c r="K51" s="1">
         <v>0.84862350075059689</v>
       </c>
-      <c r="K51" s="1">
+      <c r="L51" s="1">
         <v>0.46305975773439279</v>
       </c>
-      <c r="L51" s="1">
+      <c r="M51" s="1">
         <v>0.67472079479533198</v>
       </c>
-      <c r="M51" s="1">
+      <c r="N51" s="1">
         <v>0.32314764127687756</v>
       </c>
-      <c r="N51" s="1">
+      <c r="O51" s="1">
         <v>0.74599814143222731</v>
       </c>
-      <c r="O51" s="1">
+      <c r="P51" s="1">
         <v>0.761672911327821</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A52" s="1">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A52" s="2">
+        <v>44951</v>
+      </c>
+      <c r="B52" s="1">
         <v>0.78986596517613272</v>
       </c>
-      <c r="B52" s="1">
+      <c r="C52" s="1">
         <v>0.487864877182</v>
       </c>
-      <c r="C52" s="1">
+      <c r="D52" s="1">
         <v>0.38924032521375218</v>
       </c>
-      <c r="D52" s="1">
+      <c r="E52" s="1">
         <v>0.88233561001353222</v>
       </c>
-      <c r="E52" s="1">
+      <c r="F52" s="1">
         <v>0.11471287832837673</v>
       </c>
-      <c r="F52" s="1">
+      <c r="G52" s="1">
         <v>0.61699588024990448</v>
       </c>
-      <c r="G52" s="1">
+      <c r="H52" s="1">
         <v>0.41642728783382887</v>
       </c>
-      <c r="H52" s="1">
+      <c r="I52" s="1">
         <v>0.5648242132777832</v>
       </c>
-      <c r="I52" s="1">
+      <c r="J52" s="1">
         <v>0.68384661549404313</v>
       </c>
-      <c r="J52" s="1">
+      <c r="K52" s="1">
         <v>0.98136310195137721</v>
       </c>
-      <c r="K52" s="1">
+      <c r="L52" s="1">
         <v>0.19204498299500505</v>
       </c>
-      <c r="L52" s="1">
+      <c r="M52" s="1">
         <v>0.74782004661828927</v>
       </c>
-      <c r="M52" s="1">
+      <c r="N52" s="1">
         <v>0.6673968864313562</v>
       </c>
-      <c r="N52" s="1">
+      <c r="O52" s="1">
         <v>0.74694240429643688</v>
       </c>
-      <c r="O52" s="1">
+      <c r="P52" s="1">
         <v>0.29343175425110479</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A53" s="1">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
+        <v>44950</v>
+      </c>
+      <c r="B53" s="1">
         <v>0.72839357800044313</v>
       </c>
-      <c r="B53" s="1">
+      <c r="C53" s="1">
         <v>0.69829701834419977</v>
       </c>
-      <c r="C53" s="1">
+      <c r="D53" s="1">
         <v>0.64920186248448042</v>
       </c>
-      <c r="D53" s="1">
+      <c r="E53" s="1">
         <v>9.2447773054172067E-2</v>
       </c>
-      <c r="E53" s="1">
+      <c r="F53" s="1">
         <v>0.73624425522751413</v>
       </c>
-      <c r="F53" s="1">
+      <c r="G53" s="1">
         <v>6.5346099647915934E-2</v>
       </c>
-      <c r="G53" s="1">
+      <c r="H53" s="1">
         <v>0.2972698653111554</v>
       </c>
-      <c r="H53" s="1">
+      <c r="I53" s="1">
         <v>9.9117196602121704E-2</v>
       </c>
-      <c r="I53" s="1">
+      <c r="J53" s="1">
         <v>0.82931603313971414</v>
       </c>
-      <c r="J53" s="1">
+      <c r="K53" s="1">
         <v>0.3832213590638911</v>
       </c>
-      <c r="K53" s="1">
+      <c r="L53" s="1">
         <v>0.75817317563134912</v>
       </c>
-      <c r="L53" s="1">
+      <c r="M53" s="1">
         <v>0.33993898602241512</v>
       </c>
-      <c r="M53" s="1">
+      <c r="N53" s="1">
         <v>9.5964390064048222E-2</v>
       </c>
-      <c r="N53" s="1">
+      <c r="O53" s="1">
         <v>0.61376376063471183</v>
       </c>
-      <c r="O53" s="1">
+      <c r="P53" s="1">
         <v>0.96096084537124982</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A54" s="1">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
+        <v>44949</v>
+      </c>
+      <c r="B54" s="1">
         <v>0.76500834029914389</v>
       </c>
-      <c r="B54" s="1">
+      <c r="C54" s="1">
         <v>0.11616532018189929</v>
       </c>
-      <c r="C54" s="1">
+      <c r="D54" s="1">
         <v>0.40949873922118241</v>
       </c>
-      <c r="D54" s="1">
+      <c r="E54" s="1">
         <v>0.86747473634173011</v>
       </c>
-      <c r="E54" s="1">
+      <c r="F54" s="1">
         <v>0.24786216006197193</v>
       </c>
-      <c r="F54" s="1">
+      <c r="G54" s="1">
         <v>0.79363672612533187</v>
       </c>
-      <c r="G54" s="1">
+      <c r="H54" s="1">
         <v>0.27827204079207757</v>
       </c>
-      <c r="H54" s="1">
+      <c r="I54" s="1">
         <v>0.27784636496242787</v>
       </c>
-      <c r="I54" s="1">
+      <c r="J54" s="1">
         <v>0.30081647946792933</v>
       </c>
-      <c r="J54" s="1">
+      <c r="K54" s="1">
         <v>0.67907307400064665</v>
       </c>
-      <c r="K54" s="1">
+      <c r="L54" s="1">
         <v>0.63496324919458269</v>
       </c>
-      <c r="L54" s="1">
+      <c r="M54" s="1">
         <v>0.19576205487117992</v>
       </c>
-      <c r="M54" s="1">
+      <c r="N54" s="1">
         <v>0.61848512298573466</v>
       </c>
-      <c r="N54" s="1">
+      <c r="O54" s="1">
         <v>0.32203048113747335</v>
       </c>
-      <c r="O54" s="1">
+      <c r="P54" s="1">
         <v>0.92264730233654901</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A55" s="1">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A55" s="2">
+        <v>44948</v>
+      </c>
+      <c r="B55" s="1">
         <v>0.79088905352540284</v>
       </c>
-      <c r="B55" s="1">
+      <c r="C55" s="1">
         <v>0.60585882537998725</v>
       </c>
-      <c r="C55" s="1">
+      <c r="D55" s="1">
         <v>5.9789482928060855E-2</v>
       </c>
-      <c r="D55" s="1">
+      <c r="E55" s="1">
         <v>0.74309596321997085</v>
       </c>
-      <c r="E55" s="1">
+      <c r="F55" s="1">
         <v>0.17911237795968016</v>
       </c>
-      <c r="F55" s="1">
+      <c r="G55" s="1">
         <v>0.43338593996866526</v>
       </c>
-      <c r="G55" s="1">
+      <c r="H55" s="1">
         <v>0.20193665365480318</v>
       </c>
-      <c r="H55" s="1">
+      <c r="I55" s="1">
         <v>4.4362060855408503E-2</v>
       </c>
-      <c r="I55" s="1">
+      <c r="J55" s="1">
         <v>0.77688824949373647</v>
       </c>
-      <c r="J55" s="1">
+      <c r="K55" s="1">
         <v>0.4292794196362778</v>
       </c>
-      <c r="K55" s="1">
+      <c r="L55" s="1">
         <v>0.84413862298987075</v>
       </c>
-      <c r="L55" s="1">
+      <c r="M55" s="1">
         <v>0.64666859540833888</v>
       </c>
-      <c r="M55" s="1">
+      <c r="N55" s="1">
         <v>0.40345996967445741</v>
       </c>
-      <c r="N55" s="1">
+      <c r="O55" s="1">
         <v>8.7225405108905529E-2</v>
       </c>
-      <c r="O55" s="1">
+      <c r="P55" s="1">
         <v>0.55107384373783275</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A56" s="1">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A56" s="2">
+        <v>44947</v>
+      </c>
+      <c r="B56" s="1">
         <v>0.62244821608769973</v>
       </c>
-      <c r="B56" s="1">
+      <c r="C56" s="1">
         <v>0.79571501196404804</v>
       </c>
-      <c r="C56" s="1">
+      <c r="D56" s="1">
         <v>0.13613342607648238</v>
       </c>
-      <c r="D56" s="1">
+      <c r="E56" s="1">
         <v>0.15055586202564719</v>
       </c>
-      <c r="E56" s="1">
+      <c r="F56" s="1">
         <v>7.2676499420558649E-2</v>
       </c>
-      <c r="F56" s="1">
+      <c r="G56" s="1">
         <v>0.59831156533698859</v>
       </c>
-      <c r="G56" s="1">
+      <c r="H56" s="1">
         <v>0.29416203106283156</v>
       </c>
-      <c r="H56" s="1">
+      <c r="I56" s="1">
         <v>0.54746200954420221</v>
       </c>
-      <c r="I56" s="1">
+      <c r="J56" s="1">
         <v>0.96866442616618431</v>
       </c>
-      <c r="J56" s="1">
+      <c r="K56" s="1">
         <v>0.2872961396607514</v>
       </c>
-      <c r="K56" s="1">
+      <c r="L56" s="1">
         <v>0.97250851477075329</v>
       </c>
-      <c r="L56" s="1">
+      <c r="M56" s="1">
         <v>0.82705910535110261</v>
       </c>
-      <c r="M56" s="1">
+      <c r="N56" s="1">
         <v>0.58714297050486397</v>
       </c>
-      <c r="N56" s="1">
+      <c r="O56" s="1">
         <v>0.59163772224629607</v>
       </c>
-      <c r="O56" s="1">
+      <c r="P56" s="1">
         <v>0.92544960320735381</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A57" s="1">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A57" s="2">
+        <v>44946</v>
+      </c>
+      <c r="B57" s="1">
         <v>0.71831964003547621</v>
       </c>
-      <c r="B57" s="1">
+      <c r="C57" s="1">
         <v>0.30122582930335906</v>
       </c>
-      <c r="C57" s="1">
+      <c r="D57" s="1">
         <v>5.1803196102102045E-2</v>
       </c>
-      <c r="D57" s="1">
+      <c r="E57" s="1">
         <v>0.7668176920378097</v>
       </c>
-      <c r="E57" s="1">
+      <c r="F57" s="1">
         <v>0.33627197083640537</v>
       </c>
-      <c r="F57" s="1">
+      <c r="G57" s="1">
         <v>0.20946560471195963</v>
       </c>
-      <c r="G57" s="1">
+      <c r="H57" s="1">
         <v>9.8360445668273289E-2</v>
       </c>
-      <c r="H57" s="1">
+      <c r="I57" s="1">
         <v>0.25174793779307725</v>
       </c>
-      <c r="I57" s="1">
+      <c r="J57" s="1">
         <v>0.88235161402690554</v>
       </c>
-      <c r="J57" s="1">
+      <c r="K57" s="1">
         <v>0.81567125068276447</v>
       </c>
-      <c r="K57" s="1">
+      <c r="L57" s="1">
         <v>0.18339337247316279</v>
       </c>
-      <c r="L57" s="1">
+      <c r="M57" s="1">
         <v>0.15546976723729855</v>
       </c>
-      <c r="M57" s="1">
+      <c r="N57" s="1">
         <v>0.24697951485406566</v>
       </c>
-      <c r="N57" s="1">
+      <c r="O57" s="1">
         <v>2.7490432009578458E-2</v>
       </c>
-      <c r="O57" s="1">
+      <c r="P57" s="1">
         <v>2.3869461946671722E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A58" s="1">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A58" s="2">
+        <v>44945</v>
+      </c>
+      <c r="B58" s="1">
         <v>0.64910114940833974</v>
       </c>
-      <c r="B58" s="1">
+      <c r="C58" s="1">
         <v>0.59790338367063633</v>
       </c>
-      <c r="C58" s="1">
+      <c r="D58" s="1">
         <v>0.18287289156815745</v>
       </c>
-      <c r="D58" s="1">
+      <c r="E58" s="1">
         <v>0.71880820825245162</v>
       </c>
-      <c r="E58" s="1">
+      <c r="F58" s="1">
         <v>0.86110895317172365</v>
       </c>
-      <c r="F58" s="1">
+      <c r="G58" s="1">
         <v>0.2197010432215919</v>
       </c>
-      <c r="G58" s="1">
+      <c r="H58" s="1">
         <v>0.76805748156675357</v>
       </c>
-      <c r="H58" s="1">
+      <c r="I58" s="1">
         <v>0.11477615791412921</v>
       </c>
-      <c r="I58" s="1">
+      <c r="J58" s="1">
         <v>0.23462681372029326</v>
       </c>
-      <c r="J58" s="1">
+      <c r="K58" s="1">
         <v>0.42395278974427086</v>
       </c>
-      <c r="K58" s="1">
+      <c r="L58" s="1">
         <v>0.53526456751813134</v>
       </c>
-      <c r="L58" s="1">
+      <c r="M58" s="1">
         <v>0.39772755220025147</v>
       </c>
-      <c r="M58" s="1">
+      <c r="N58" s="1">
         <v>0.27935237304224747</v>
       </c>
-      <c r="N58" s="1">
+      <c r="O58" s="1">
         <v>0.10715885238707734</v>
       </c>
-      <c r="O58" s="1">
+      <c r="P58" s="1">
         <v>0.52791518722839192</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A59" s="1">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A59" s="2">
+        <v>44944</v>
+      </c>
+      <c r="B59" s="1">
         <v>0.16861419377939146</v>
       </c>
-      <c r="B59" s="1">
+      <c r="C59" s="1">
         <v>0.2167072747604496</v>
       </c>
-      <c r="C59" s="1">
+      <c r="D59" s="1">
         <v>0.17413185242754403</v>
       </c>
-      <c r="D59" s="1">
+      <c r="E59" s="1">
         <v>9.1833673922537051E-2</v>
       </c>
-      <c r="E59" s="1">
+      <c r="F59" s="1">
         <v>0.37839776119975821</v>
       </c>
-      <c r="F59" s="1">
+      <c r="G59" s="1">
         <v>0.83410167898519105</v>
       </c>
-      <c r="G59" s="1">
+      <c r="H59" s="1">
         <v>0.37232901207391056</v>
       </c>
-      <c r="H59" s="1">
+      <c r="I59" s="1">
         <v>0.33659445587859416</v>
       </c>
-      <c r="I59" s="1">
+      <c r="J59" s="1">
         <v>0.96215553076588334</v>
       </c>
-      <c r="J59" s="1">
+      <c r="K59" s="1">
         <v>0.58840852868396099</v>
       </c>
-      <c r="K59" s="1">
+      <c r="L59" s="1">
         <v>0.31589806576968571</v>
       </c>
-      <c r="L59" s="1">
+      <c r="M59" s="1">
         <v>0.90961772562040244</v>
       </c>
-      <c r="M59" s="1">
+      <c r="N59" s="1">
         <v>0.97636498301994457</v>
       </c>
-      <c r="N59" s="1">
+      <c r="O59" s="1">
         <v>0.50571974710248269</v>
       </c>
-      <c r="O59" s="1">
+      <c r="P59" s="1">
         <v>0.93175205740614886</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A60" s="1">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A60" s="2">
+        <v>44943</v>
+      </c>
+      <c r="B60" s="1">
         <v>0.4274885558400201</v>
       </c>
-      <c r="B60" s="1">
+      <c r="C60" s="1">
         <v>0.85069390643004195</v>
       </c>
-      <c r="C60" s="1">
+      <c r="D60" s="1">
         <v>0.93611576185850121</v>
       </c>
-      <c r="D60" s="1">
+      <c r="E60" s="1">
         <v>0.90782780887902015</v>
       </c>
-      <c r="E60" s="1">
+      <c r="F60" s="1">
         <v>0.20577750175547438</v>
       </c>
-      <c r="F60" s="1">
+      <c r="G60" s="1">
         <v>0.50035929247915267</v>
       </c>
-      <c r="G60" s="1">
+      <c r="H60" s="1">
         <v>0.54607666995486381</v>
       </c>
-      <c r="H60" s="1">
+      <c r="I60" s="1">
         <v>0.93476750761642069</v>
       </c>
-      <c r="I60" s="1">
+      <c r="J60" s="1">
         <v>0.2099954015431954</v>
       </c>
-      <c r="J60" s="1">
+      <c r="K60" s="1">
         <v>0.25543658325730201</v>
       </c>
-      <c r="K60" s="1">
+      <c r="L60" s="1">
         <v>0.57688939528238836</v>
       </c>
-      <c r="L60" s="1">
+      <c r="M60" s="1">
         <v>0.15388338114640943</v>
       </c>
-      <c r="M60" s="1">
+      <c r="N60" s="1">
         <v>0.44759317663587173</v>
       </c>
-      <c r="N60" s="1">
+      <c r="O60" s="1">
         <v>7.0435539615775977E-2</v>
       </c>
-      <c r="O60" s="1">
+      <c r="P60" s="1">
         <v>0.859287391693767</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A61" s="1">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A61" s="2">
+        <v>44942</v>
+      </c>
+      <c r="B61" s="1">
         <v>0.20008504196563404</v>
       </c>
-      <c r="B61" s="1">
+      <c r="C61" s="1">
         <v>0.77502980292418544</v>
       </c>
-      <c r="C61" s="1">
+      <c r="D61" s="1">
         <v>0.11701832597190986</v>
       </c>
-      <c r="D61" s="1">
+      <c r="E61" s="1">
         <v>0.51496480082871365</v>
       </c>
-      <c r="E61" s="1">
+      <c r="F61" s="1">
         <v>0.19127559249153037</v>
       </c>
-      <c r="F61" s="1">
+      <c r="G61" s="1">
         <v>0.30699962055159125</v>
       </c>
-      <c r="G61" s="1">
+      <c r="H61" s="1">
         <v>0.23468305654222699</v>
       </c>
-      <c r="H61" s="1">
+      <c r="I61" s="1">
         <v>0.43656642050970862</v>
       </c>
-      <c r="I61" s="1">
+      <c r="J61" s="1">
         <v>0.31354797772784049</v>
       </c>
-      <c r="J61" s="1">
+      <c r="K61" s="1">
         <v>0.32003240991493942</v>
       </c>
-      <c r="K61" s="1">
+      <c r="L61" s="1">
         <v>0.28050960409329151</v>
       </c>
-      <c r="L61" s="1">
+      <c r="M61" s="1">
         <v>0.53951181788986924</v>
       </c>
-      <c r="M61" s="1">
+      <c r="N61" s="1">
         <v>0.16897287155231688</v>
       </c>
-      <c r="N61" s="1">
+      <c r="O61" s="1">
         <v>0.75150171632104024</v>
       </c>
-      <c r="O61" s="1">
+      <c r="P61" s="1">
         <v>0.24093028733181376</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A62" s="1">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A62" s="2">
+        <v>44941</v>
+      </c>
+      <c r="B62" s="1">
         <v>0.88909419635349263</v>
       </c>
-      <c r="B62" s="1">
+      <c r="C62" s="1">
         <v>0.26669755189983124</v>
       </c>
-      <c r="C62" s="1">
+      <c r="D62" s="1">
         <v>0.75353136423607525</v>
       </c>
-      <c r="D62" s="1">
+      <c r="E62" s="1">
         <v>9.9027559143077926E-2</v>
       </c>
-      <c r="E62" s="1">
+      <c r="F62" s="1">
         <v>0.43496679975812003</v>
       </c>
-      <c r="F62" s="1">
+      <c r="G62" s="1">
         <v>0.80386540074310597</v>
       </c>
-      <c r="G62" s="1">
+      <c r="H62" s="1">
         <v>0.98128279272854635</v>
       </c>
-      <c r="H62" s="1">
+      <c r="I62" s="1">
         <v>0.92133158546125682</v>
       </c>
-      <c r="I62" s="1">
+      <c r="J62" s="1">
         <v>0.11321032240024897</v>
       </c>
-      <c r="J62" s="1">
+      <c r="K62" s="1">
         <v>0.47674944422384591</v>
       </c>
-      <c r="K62" s="1">
+      <c r="L62" s="1">
         <v>0.12691815689259267</v>
       </c>
-      <c r="L62" s="1">
+      <c r="M62" s="1">
         <v>0.78004914446835827</v>
       </c>
-      <c r="M62" s="1">
+      <c r="N62" s="1">
         <v>0.85909973423022135</v>
       </c>
-      <c r="N62" s="1">
+      <c r="O62" s="1">
         <v>0.49429844765708641</v>
       </c>
-      <c r="O62" s="1">
+      <c r="P62" s="1">
         <v>0.3810071926184454</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A63" s="1">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A63" s="2">
+        <v>44940</v>
+      </c>
+      <c r="B63" s="1">
         <v>0.26196784065662637</v>
       </c>
-      <c r="B63" s="1">
+      <c r="C63" s="1">
         <v>0.22764437666255266</v>
       </c>
-      <c r="C63" s="1">
+      <c r="D63" s="1">
         <v>0.43163596432995988</v>
       </c>
-      <c r="D63" s="1">
+      <c r="E63" s="1">
         <v>0.4480617553765216</v>
       </c>
-      <c r="E63" s="1">
+      <c r="F63" s="1">
         <v>0.49182286681247822</v>
       </c>
-      <c r="F63" s="1">
+      <c r="G63" s="1">
         <v>0.24861155171477267</v>
       </c>
-      <c r="G63" s="1">
+      <c r="H63" s="1">
         <v>0.7463188492482663</v>
       </c>
-      <c r="H63" s="1">
+      <c r="I63" s="1">
         <v>0.71917797780466441</v>
       </c>
-      <c r="I63" s="1">
+      <c r="J63" s="1">
         <v>0.30239558783897658</v>
       </c>
-      <c r="J63" s="1">
+      <c r="K63" s="1">
         <v>0.55818714691929494</v>
       </c>
-      <c r="K63" s="1">
+      <c r="L63" s="1">
         <v>0.67030988959041216</v>
       </c>
-      <c r="L63" s="1">
+      <c r="M63" s="1">
         <v>0.92802806693425688</v>
       </c>
-      <c r="M63" s="1">
+      <c r="N63" s="1">
         <v>0.51062210841303235</v>
       </c>
-      <c r="N63" s="1">
+      <c r="O63" s="1">
         <v>0.13444744369121497</v>
       </c>
-      <c r="O63" s="1">
+      <c r="P63" s="1">
         <v>0.85051285133680399</v>
       </c>
     </row>

</xml_diff>